<commit_message>
added - data and edit scripts
</commit_message>
<xml_diff>
--- a/analyses/pilotData_all.xlsx
+++ b/analyses/pilotData_all.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://istitutoitalianotecnologia-my.sharepoint.com/personal/mariacarla_memeo_iit_it/Documents/Documents/GitHub/joint-motor-decision/analyses/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MMemeo\OneDrive - Fondazione Istituto Italiano Tecnologia\Documents\GitHub\joint-motor-decision\analyses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DDF43D61-AFCC-4082-8C81-786064A4A95A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{DDF43D61-AFCC-4082-8C81-786064A4A95A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{0ECF3D4A-0F7C-415D-88F8-A8CA1D5DB54B}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13860" windowHeight="9330" activeTab="3" xr2:uid="{A80D8D59-C096-4587-A6C8-4C0B6ECCC775}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13860" windowHeight="9330" xr2:uid="{A80D8D59-C096-4587-A6C8-4C0B6ECCC775}"/>
   </bookViews>
   <sheets>
     <sheet name="P100" sheetId="1" r:id="rId1"/>
@@ -484,11 +484,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D8BE86-51E1-4E35-A1FE-0679F1EDE2B0}">
   <dimension ref="A1:AH160"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection sqref="A1:AH160"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AH4" sqref="AH4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" customWidth="1"/>
+    <col min="9" max="9" width="7.140625" customWidth="1"/>
+    <col min="10" max="10" width="5.85546875" customWidth="1"/>
+    <col min="11" max="11" width="6.85546875" customWidth="1"/>
+    <col min="12" max="12" width="8.28515625" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" customWidth="1"/>
+    <col min="14" max="14" width="11.85546875" customWidth="1"/>
+    <col min="15" max="15" width="7.140625" customWidth="1"/>
+    <col min="16" max="16" width="5.85546875" customWidth="1"/>
+    <col min="17" max="17" width="6.85546875" customWidth="1"/>
+    <col min="18" max="18" width="8.28515625" customWidth="1"/>
+    <col min="19" max="19" width="10.42578125" customWidth="1"/>
+    <col min="20" max="20" width="13" customWidth="1"/>
+    <col min="21" max="21" width="8.28515625" customWidth="1"/>
+    <col min="22" max="22" width="7" customWidth="1"/>
+    <col min="23" max="23" width="8" customWidth="1"/>
+    <col min="24" max="24" width="9.42578125" customWidth="1"/>
+    <col min="25" max="25" width="11.5703125" customWidth="1"/>
+    <col min="26" max="26" width="23.5703125" customWidth="1"/>
+    <col min="27" max="27" width="26.140625" customWidth="1"/>
+    <col min="28" max="28" width="23.140625" customWidth="1"/>
+    <col min="29" max="29" width="13.7109375" style="1" customWidth="1"/>
+    <col min="30" max="30" width="12.7109375" style="1" customWidth="1"/>
+    <col min="31" max="31" width="13.7109375" style="1" customWidth="1"/>
+    <col min="32" max="34" width="12.7109375" style="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -575,22 +609,22 @@
       <c r="AB1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>33</v>
       </c>
     </row>
@@ -679,22 +713,22 @@
       <c r="AB2">
         <v>1</v>
       </c>
-      <c r="AC2">
+      <c r="AC2" s="1">
         <v>0.52999997138977051</v>
       </c>
-      <c r="AD2">
+      <c r="AD2" s="1">
         <v>0.97000002861022949</v>
       </c>
-      <c r="AE2">
+      <c r="AE2" s="1">
         <v>0.57999998331069946</v>
       </c>
-      <c r="AF2">
+      <c r="AF2" s="1">
         <v>0.57999998331069946</v>
       </c>
-      <c r="AG2">
+      <c r="AG2" s="1">
         <v>1.0900000333786011</v>
       </c>
-      <c r="AH2">
+      <c r="AH2" s="1">
         <v>0.56999999284744263</v>
       </c>
     </row>
@@ -783,16 +817,16 @@
       <c r="AB3">
         <v>2</v>
       </c>
-      <c r="AC3">
+      <c r="AC3" s="1">
         <v>0.82999998331069946</v>
       </c>
-      <c r="AE3">
+      <c r="AE3" s="1">
         <v>1.0900000333786011</v>
       </c>
-      <c r="AF3">
+      <c r="AF3" s="1">
         <v>0.76999998092651367</v>
       </c>
-      <c r="AH3">
+      <c r="AH3" s="1">
         <v>0.68999999761581421</v>
       </c>
     </row>
@@ -881,10 +915,10 @@
       <c r="AB4">
         <v>1</v>
       </c>
-      <c r="AD4">
+      <c r="AD4" s="1">
         <v>1.1499999761581421</v>
       </c>
-      <c r="AG4">
+      <c r="AG4" s="1">
         <v>1.1399999856948853</v>
       </c>
     </row>
@@ -973,22 +1007,22 @@
       <c r="AB5">
         <v>2</v>
       </c>
-      <c r="AC5">
+      <c r="AC5" s="1">
         <v>0.57999998331069946</v>
       </c>
-      <c r="AD5">
+      <c r="AD5" s="1">
         <v>0.98000001907348633</v>
       </c>
-      <c r="AE5">
+      <c r="AE5" s="1">
         <v>0.85000002384185791</v>
       </c>
-      <c r="AF5">
+      <c r="AF5" s="1">
         <v>0.77999997138977051</v>
       </c>
-      <c r="AG5">
+      <c r="AG5" s="1">
         <v>0.57999998331069946</v>
       </c>
-      <c r="AH5">
+      <c r="AH5" s="1">
         <v>0.9100000262260437</v>
       </c>
     </row>
@@ -1077,16 +1111,16 @@
       <c r="AB6">
         <v>1</v>
       </c>
-      <c r="AD6">
+      <c r="AD6" s="1">
         <v>0.14000000059604645</v>
       </c>
-      <c r="AE6">
+      <c r="AE6" s="1">
         <v>0.50999999046325684</v>
       </c>
-      <c r="AG6">
+      <c r="AG6" s="1">
         <v>0.79000002145767212</v>
       </c>
-      <c r="AH6">
+      <c r="AH6" s="1">
         <v>0.56999999284744263</v>
       </c>
     </row>
@@ -1175,16 +1209,16 @@
       <c r="AB7">
         <v>2</v>
       </c>
-      <c r="AC7">
+      <c r="AC7" s="1">
         <v>0.81000000238418579</v>
       </c>
-      <c r="AE7">
+      <c r="AE7" s="1">
         <v>2.6500000953674316</v>
       </c>
-      <c r="AF7">
+      <c r="AF7" s="1">
         <v>0.75999999046325684</v>
       </c>
-      <c r="AH7">
+      <c r="AH7" s="1">
         <v>0.72000002861022949</v>
       </c>
     </row>
@@ -1273,16 +1307,16 @@
       <c r="AB8">
         <v>1</v>
       </c>
-      <c r="AD8">
+      <c r="AD8" s="1">
         <v>1.75</v>
       </c>
-      <c r="AE8">
+      <c r="AE8" s="1">
         <v>0.60000002384185791</v>
       </c>
-      <c r="AG8">
+      <c r="AG8" s="1">
         <v>0.87999999523162842</v>
       </c>
-      <c r="AH8">
+      <c r="AH8" s="1">
         <v>0.47999998927116394</v>
       </c>
     </row>
@@ -1371,16 +1405,16 @@
       <c r="AB9">
         <v>2</v>
       </c>
-      <c r="AC9">
+      <c r="AC9" s="1">
         <v>1.1599999666213989</v>
       </c>
-      <c r="AE9">
+      <c r="AE9" s="1">
         <v>2.4800000190734863</v>
       </c>
-      <c r="AF9">
+      <c r="AF9" s="1">
         <v>0.94999998807907104</v>
       </c>
-      <c r="AH9">
+      <c r="AH9" s="1">
         <v>0.85000002384185791</v>
       </c>
     </row>
@@ -1469,16 +1503,16 @@
       <c r="AB10">
         <v>1</v>
       </c>
-      <c r="AD10">
+      <c r="AD10" s="1">
         <v>1.1499999761581421</v>
       </c>
-      <c r="AE10">
+      <c r="AE10" s="1">
         <v>0.75999999046325684</v>
       </c>
-      <c r="AG10">
+      <c r="AG10" s="1">
         <v>1.0900000333786011</v>
       </c>
-      <c r="AH10">
+      <c r="AH10" s="1">
         <v>0.72000002861022949</v>
       </c>
     </row>
@@ -1567,22 +1601,22 @@
       <c r="AB11">
         <v>2</v>
       </c>
-      <c r="AC11">
+      <c r="AC11" s="1">
         <v>1.3400000333786011</v>
       </c>
-      <c r="AD11">
+      <c r="AD11" s="1">
         <v>1.8600000143051147</v>
       </c>
-      <c r="AE11">
+      <c r="AE11" s="1">
         <v>0.20000000298023224</v>
       </c>
-      <c r="AF11">
+      <c r="AF11" s="1">
         <v>1.25</v>
       </c>
-      <c r="AG11">
+      <c r="AG11" s="1">
         <v>0.68000000715255737</v>
       </c>
-      <c r="AH11">
+      <c r="AH11" s="1">
         <v>1.8700000047683716</v>
       </c>
     </row>
@@ -1671,22 +1705,22 @@
       <c r="AB12">
         <v>1</v>
       </c>
-      <c r="AC12">
+      <c r="AC12" s="1">
         <v>0.55000001192092896</v>
       </c>
-      <c r="AD12">
+      <c r="AD12" s="1">
         <v>0.37999999523162842</v>
       </c>
-      <c r="AE12">
+      <c r="AE12" s="1">
         <v>0.70999997854232788</v>
       </c>
-      <c r="AF12">
+      <c r="AF12" s="1">
         <v>0.64999997615814209</v>
       </c>
-      <c r="AG12">
+      <c r="AG12" s="1">
         <v>0.81999999284744263</v>
       </c>
-      <c r="AH12">
+      <c r="AH12" s="1">
         <v>0.47999998927116394</v>
       </c>
     </row>
@@ -1775,22 +1809,22 @@
       <c r="AB13">
         <v>2</v>
       </c>
-      <c r="AC13">
+      <c r="AC13" s="1">
         <v>0.62000000476837158</v>
       </c>
-      <c r="AD13">
+      <c r="AD13" s="1">
         <v>1.0399999618530273</v>
       </c>
-      <c r="AE13">
+      <c r="AE13" s="1">
         <v>0.4699999988079071</v>
       </c>
-      <c r="AF13">
+      <c r="AF13" s="1">
         <v>1.0399999618530273</v>
       </c>
-      <c r="AG13">
+      <c r="AG13" s="1">
         <v>0.63999998569488525</v>
       </c>
-      <c r="AH13">
+      <c r="AH13" s="1">
         <v>0.77999997138977051</v>
       </c>
     </row>
@@ -1879,22 +1913,22 @@
       <c r="AB14">
         <v>1</v>
       </c>
-      <c r="AC14">
+      <c r="AC14" s="1">
         <v>1.0099999904632568</v>
       </c>
-      <c r="AD14">
+      <c r="AD14" s="1">
         <v>0.25999999046325684</v>
       </c>
-      <c r="AE14">
+      <c r="AE14" s="1">
         <v>0.70999997854232788</v>
       </c>
-      <c r="AF14">
+      <c r="AF14" s="1">
         <v>0.62999999523162842</v>
       </c>
-      <c r="AG14">
+      <c r="AG14" s="1">
         <v>0.5899999737739563</v>
       </c>
-      <c r="AH14">
+      <c r="AH14" s="1">
         <v>0.49000000953674316</v>
       </c>
     </row>
@@ -1983,22 +2017,22 @@
       <c r="AB15">
         <v>2</v>
       </c>
-      <c r="AC15">
+      <c r="AC15" s="1">
         <v>0.2199999988079071</v>
       </c>
-      <c r="AD15">
+      <c r="AD15" s="1">
         <v>0.4699999988079071</v>
       </c>
-      <c r="AE15">
+      <c r="AE15" s="1">
         <v>0.40000000596046448</v>
       </c>
-      <c r="AF15">
+      <c r="AF15" s="1">
         <v>0.80000001192092896</v>
       </c>
-      <c r="AG15">
+      <c r="AG15" s="1">
         <v>0.56000000238418579</v>
       </c>
-      <c r="AH15">
+      <c r="AH15" s="1">
         <v>0.73000001907348633</v>
       </c>
     </row>
@@ -2087,22 +2121,22 @@
       <c r="AB16">
         <v>1</v>
       </c>
-      <c r="AC16">
+      <c r="AC16" s="1">
         <v>1.7200000286102295</v>
       </c>
-      <c r="AD16">
+      <c r="AD16" s="1">
         <v>0.98000001907348633</v>
       </c>
-      <c r="AE16">
+      <c r="AE16" s="1">
         <v>0.36000001430511475</v>
       </c>
-      <c r="AF16">
+      <c r="AF16" s="1">
         <v>0.5</v>
       </c>
-      <c r="AG16">
+      <c r="AG16" s="1">
         <v>1.2899999618530273</v>
       </c>
-      <c r="AH16">
+      <c r="AH16" s="1">
         <v>0.52999997138977051</v>
       </c>
     </row>
@@ -2191,22 +2225,22 @@
       <c r="AB17">
         <v>2</v>
       </c>
-      <c r="AC17">
+      <c r="AC17" s="1">
         <v>0.30000001192092896</v>
       </c>
-      <c r="AD17">
+      <c r="AD17" s="1">
         <v>1.8700000047683716</v>
       </c>
-      <c r="AE17">
+      <c r="AE17" s="1">
         <v>0.75</v>
       </c>
-      <c r="AF17">
+      <c r="AF17" s="1">
         <v>1.3400000333786011</v>
       </c>
-      <c r="AG17">
+      <c r="AG17" s="1">
         <v>0.56999999284744263</v>
       </c>
-      <c r="AH17">
+      <c r="AH17" s="1">
         <v>0.74000000953674316</v>
       </c>
     </row>
@@ -2295,22 +2329,22 @@
       <c r="AB18">
         <v>1</v>
       </c>
-      <c r="AC18">
+      <c r="AC18" s="1">
         <v>0.41999998688697815</v>
       </c>
-      <c r="AD18">
+      <c r="AD18" s="1">
         <v>0.6600000262260437</v>
       </c>
-      <c r="AE18">
+      <c r="AE18" s="1">
         <v>0.37000000476837158</v>
       </c>
-      <c r="AF18">
+      <c r="AF18" s="1">
         <v>0.56999999284744263</v>
       </c>
-      <c r="AG18">
+      <c r="AG18" s="1">
         <v>0.72000002861022949</v>
       </c>
-      <c r="AH18">
+      <c r="AH18" s="1">
         <v>0.49000000953674316</v>
       </c>
     </row>
@@ -2399,22 +2433,22 @@
       <c r="AB19">
         <v>2</v>
       </c>
-      <c r="AC19">
+      <c r="AC19" s="1">
         <v>1.9299999475479126</v>
       </c>
-      <c r="AD19">
+      <c r="AD19" s="1">
         <v>1.2999999523162842</v>
       </c>
-      <c r="AE19">
+      <c r="AE19" s="1">
         <v>0.50999999046325684</v>
       </c>
-      <c r="AF19">
+      <c r="AF19" s="1">
         <v>1.0800000429153442</v>
       </c>
-      <c r="AG19">
+      <c r="AG19" s="1">
         <v>0.69999998807907104</v>
       </c>
-      <c r="AH19">
+      <c r="AH19" s="1">
         <v>0.86000001430511475</v>
       </c>
     </row>
@@ -2503,22 +2537,22 @@
       <c r="AB20">
         <v>1</v>
       </c>
-      <c r="AC20">
+      <c r="AC20" s="1">
         <v>1.2599999904632568</v>
       </c>
-      <c r="AD20">
+      <c r="AD20" s="1">
         <v>0.4699999988079071</v>
       </c>
-      <c r="AE20">
+      <c r="AE20" s="1">
         <v>0.47999998927116394</v>
       </c>
-      <c r="AF20">
+      <c r="AF20" s="1">
         <v>0.85000002384185791</v>
       </c>
-      <c r="AG20">
+      <c r="AG20" s="1">
         <v>0.9100000262260437</v>
       </c>
-      <c r="AH20">
+      <c r="AH20" s="1">
         <v>0.68000000715255737</v>
       </c>
     </row>
@@ -2607,22 +2641,22 @@
       <c r="AB21">
         <v>2</v>
       </c>
-      <c r="AC21">
+      <c r="AC21" s="1">
         <v>1.9700000286102295</v>
       </c>
-      <c r="AD21">
+      <c r="AD21" s="1">
         <v>1.5199999809265137</v>
       </c>
-      <c r="AE21">
+      <c r="AE21" s="1">
         <v>2.6700000762939453</v>
       </c>
-      <c r="AF21">
+      <c r="AF21" s="1">
         <v>1.0900000333786011</v>
       </c>
-      <c r="AG21">
+      <c r="AG21" s="1">
         <v>0.63999998569488525</v>
       </c>
-      <c r="AH21">
+      <c r="AH21" s="1">
         <v>0.81000000238418579</v>
       </c>
     </row>
@@ -2711,22 +2745,22 @@
       <c r="AB22">
         <v>1</v>
       </c>
-      <c r="AC22">
+      <c r="AC22" s="1">
         <v>2.0199999809265137</v>
       </c>
-      <c r="AD22">
+      <c r="AD22" s="1">
         <v>0.20999999344348907</v>
       </c>
-      <c r="AE22">
+      <c r="AE22" s="1">
         <v>0.50999999046325684</v>
       </c>
-      <c r="AF22">
+      <c r="AF22" s="1">
         <v>0.86000001430511475</v>
       </c>
-      <c r="AG22">
+      <c r="AG22" s="1">
         <v>0.5899999737739563</v>
       </c>
-      <c r="AH22">
+      <c r="AH22" s="1">
         <v>0.52999997138977051</v>
       </c>
     </row>
@@ -2815,22 +2849,22 @@
       <c r="AB23">
         <v>2</v>
       </c>
-      <c r="AC23">
+      <c r="AC23" s="1">
         <v>0.54000002145767212</v>
       </c>
-      <c r="AD23">
+      <c r="AD23" s="1">
         <v>1.7699999809265137</v>
       </c>
-      <c r="AE23">
+      <c r="AE23" s="1">
         <v>1.9299999475479126</v>
       </c>
-      <c r="AF23">
+      <c r="AF23" s="1">
         <v>0.88999998569488525</v>
       </c>
-      <c r="AG23">
+      <c r="AG23" s="1">
         <v>1.0099999904632568</v>
       </c>
-      <c r="AH23">
+      <c r="AH23" s="1">
         <v>1</v>
       </c>
     </row>
@@ -2919,22 +2953,22 @@
       <c r="AB24">
         <v>1</v>
       </c>
-      <c r="AC24">
+      <c r="AC24" s="1">
         <v>1.4600000381469727</v>
       </c>
-      <c r="AD24">
+      <c r="AD24" s="1">
         <v>0.51999998092651367</v>
       </c>
-      <c r="AE24">
+      <c r="AE24" s="1">
         <v>0.37000000476837158</v>
       </c>
-      <c r="AF24">
+      <c r="AF24" s="1">
         <v>0.54000002145767212</v>
       </c>
-      <c r="AG24">
+      <c r="AG24" s="1">
         <v>1.0099999904632568</v>
       </c>
-      <c r="AH24">
+      <c r="AH24" s="1">
         <v>0.62000000476837158</v>
       </c>
     </row>
@@ -3023,22 +3057,22 @@
       <c r="AB25">
         <v>2</v>
       </c>
-      <c r="AC25">
+      <c r="AC25" s="1">
         <v>0.18000000715255737</v>
       </c>
-      <c r="AD25">
+      <c r="AD25" s="1">
         <v>2.380000114440918</v>
       </c>
-      <c r="AE25">
+      <c r="AE25" s="1">
         <v>1.0099999904632568</v>
       </c>
-      <c r="AF25">
+      <c r="AF25" s="1">
         <v>1.0199999809265137</v>
       </c>
-      <c r="AG25">
+      <c r="AG25" s="1">
         <v>0.8399999737739563</v>
       </c>
-      <c r="AH25">
+      <c r="AH25" s="1">
         <v>1.3500000238418579</v>
       </c>
     </row>
@@ -3127,16 +3161,16 @@
       <c r="AB26">
         <v>1</v>
       </c>
-      <c r="AC26">
+      <c r="AC26" s="1">
         <v>0.25</v>
       </c>
-      <c r="AE26">
+      <c r="AE26" s="1">
         <v>0.40000000596046448</v>
       </c>
-      <c r="AF26">
+      <c r="AF26" s="1">
         <v>0.61000001430511475</v>
       </c>
-      <c r="AH26">
+      <c r="AH26" s="1">
         <v>0.68999999761581421</v>
       </c>
     </row>
@@ -3225,22 +3259,22 @@
       <c r="AB27">
         <v>2</v>
       </c>
-      <c r="AC27">
+      <c r="AC27" s="1">
         <v>0.57999998331069946</v>
       </c>
-      <c r="AD27">
+      <c r="AD27" s="1">
         <v>1.7300000190734863</v>
       </c>
-      <c r="AE27">
+      <c r="AE27" s="1">
         <v>0.81000000238418579</v>
       </c>
-      <c r="AF27">
+      <c r="AF27" s="1">
         <v>1.0299999713897705</v>
       </c>
-      <c r="AG27">
+      <c r="AG27" s="1">
         <v>0.97000002861022949</v>
       </c>
-      <c r="AH27">
+      <c r="AH27" s="1">
         <v>0.67000001668930054</v>
       </c>
     </row>
@@ -3329,22 +3363,22 @@
       <c r="AB28">
         <v>1</v>
       </c>
-      <c r="AC28">
+      <c r="AC28" s="1">
         <v>1.4299999475479126</v>
       </c>
-      <c r="AD28">
+      <c r="AD28" s="1">
         <v>2.2899999618530273</v>
       </c>
-      <c r="AE28">
+      <c r="AE28" s="1">
         <v>1.2400000095367432</v>
       </c>
-      <c r="AF28">
+      <c r="AF28" s="1">
         <v>0.67000001668930054</v>
       </c>
-      <c r="AG28">
+      <c r="AG28" s="1">
         <v>0.99000000953674316</v>
       </c>
-      <c r="AH28">
+      <c r="AH28" s="1">
         <v>0.68000000715255737</v>
       </c>
     </row>
@@ -3433,22 +3467,22 @@
       <c r="AB29">
         <v>2</v>
       </c>
-      <c r="AC29">
+      <c r="AC29" s="1">
         <v>1.4199999570846558</v>
       </c>
-      <c r="AD29">
+      <c r="AD29" s="1">
         <v>0.4699999988079071</v>
       </c>
-      <c r="AE29">
+      <c r="AE29" s="1">
         <v>0.77999997138977051</v>
       </c>
-      <c r="AF29">
+      <c r="AF29" s="1">
         <v>1.6299999952316284</v>
       </c>
-      <c r="AG29">
+      <c r="AG29" s="1">
         <v>0.60000002384185791</v>
       </c>
-      <c r="AH29">
+      <c r="AH29" s="1">
         <v>0.75999999046325684</v>
       </c>
     </row>
@@ -3537,22 +3571,22 @@
       <c r="AB30">
         <v>1</v>
       </c>
-      <c r="AC30">
+      <c r="AC30" s="1">
         <v>2.3599998950958252</v>
       </c>
-      <c r="AD30">
+      <c r="AD30" s="1">
         <v>0.5899999737739563</v>
       </c>
-      <c r="AE30">
+      <c r="AE30" s="1">
         <v>0.47999998927116394</v>
       </c>
-      <c r="AF30">
+      <c r="AF30" s="1">
         <v>1.4099999666213989</v>
       </c>
-      <c r="AG30">
+      <c r="AG30" s="1">
         <v>1.1699999570846558</v>
       </c>
-      <c r="AH30">
+      <c r="AH30" s="1">
         <v>0.60000002384185791</v>
       </c>
     </row>
@@ -3641,22 +3675,22 @@
       <c r="AB31">
         <v>2</v>
       </c>
-      <c r="AC31">
+      <c r="AC31" s="1">
         <v>0.25</v>
       </c>
-      <c r="AD31">
+      <c r="AD31" s="1">
         <v>2.7100000381469727</v>
       </c>
-      <c r="AE31">
+      <c r="AE31" s="1">
         <v>0.94999998807907104</v>
       </c>
-      <c r="AF31">
+      <c r="AF31" s="1">
         <v>0.63999998569488525</v>
       </c>
-      <c r="AG31">
+      <c r="AG31" s="1">
         <v>0.85000002384185791</v>
       </c>
-      <c r="AH31">
+      <c r="AH31" s="1">
         <v>0.76999998092651367</v>
       </c>
     </row>
@@ -3745,22 +3779,22 @@
       <c r="AB32">
         <v>1</v>
       </c>
-      <c r="AC32">
+      <c r="AC32" s="1">
         <v>0.18000000715255737</v>
       </c>
-      <c r="AD32">
+      <c r="AD32" s="1">
         <v>0.25999999046325684</v>
       </c>
-      <c r="AE32">
+      <c r="AE32" s="1">
         <v>5.9999998658895493E-2</v>
       </c>
-      <c r="AF32">
+      <c r="AF32" s="1">
         <v>0.60000002384185791</v>
       </c>
-      <c r="AG32">
+      <c r="AG32" s="1">
         <v>0.88999998569488525</v>
       </c>
-      <c r="AH32">
+      <c r="AH32" s="1">
         <v>0.86000001430511475</v>
       </c>
     </row>
@@ -3849,22 +3883,22 @@
       <c r="AB33">
         <v>2</v>
       </c>
-      <c r="AC33">
+      <c r="AC33" s="1">
         <v>0.34999999403953552</v>
       </c>
-      <c r="AD33">
+      <c r="AD33" s="1">
         <v>1.7200000286102295</v>
       </c>
-      <c r="AE33">
+      <c r="AE33" s="1">
         <v>0.63999998569488525</v>
       </c>
-      <c r="AF33">
+      <c r="AF33" s="1">
         <v>0.75999999046325684</v>
       </c>
-      <c r="AG33">
-        <v>1</v>
-      </c>
-      <c r="AH33">
+      <c r="AG33" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH33" s="1">
         <v>0.70999997854232788</v>
       </c>
     </row>
@@ -3953,22 +3987,22 @@
       <c r="AB34">
         <v>1</v>
       </c>
-      <c r="AC34">
+      <c r="AC34" s="1">
         <v>0.94999998807907104</v>
       </c>
-      <c r="AD34">
+      <c r="AD34" s="1">
         <v>1.2899999618530273</v>
       </c>
-      <c r="AE34">
+      <c r="AE34" s="1">
         <v>0.25</v>
       </c>
-      <c r="AF34">
+      <c r="AF34" s="1">
         <v>0.75999999046325684</v>
       </c>
-      <c r="AG34">
+      <c r="AG34" s="1">
         <v>1.2000000476837158</v>
       </c>
-      <c r="AH34">
+      <c r="AH34" s="1">
         <v>0.79000002145767212</v>
       </c>
     </row>
@@ -4057,22 +4091,22 @@
       <c r="AB35">
         <v>2</v>
       </c>
-      <c r="AC35">
+      <c r="AC35" s="1">
         <v>0.75</v>
       </c>
-      <c r="AD35">
+      <c r="AD35" s="1">
         <v>1.6100000143051147</v>
       </c>
-      <c r="AE35">
+      <c r="AE35" s="1">
         <v>1.3899999856948853</v>
       </c>
-      <c r="AF35">
+      <c r="AF35" s="1">
         <v>1.9700000286102295</v>
       </c>
-      <c r="AG35">
+      <c r="AG35" s="1">
         <v>1.0299999713897705</v>
       </c>
-      <c r="AH35">
+      <c r="AH35" s="1">
         <v>1.3400000333786011</v>
       </c>
     </row>
@@ -4161,22 +4195,22 @@
       <c r="AB36">
         <v>1</v>
       </c>
-      <c r="AC36">
+      <c r="AC36" s="1">
         <v>0.20999999344348907</v>
       </c>
-      <c r="AD36">
+      <c r="AD36" s="1">
         <v>1.25</v>
       </c>
-      <c r="AE36">
+      <c r="AE36" s="1">
         <v>0.23999999463558197</v>
       </c>
-      <c r="AF36">
+      <c r="AF36" s="1">
         <v>0.68000000715255737</v>
       </c>
-      <c r="AG36">
+      <c r="AG36" s="1">
         <v>1.2599999904632568</v>
       </c>
-      <c r="AH36">
+      <c r="AH36" s="1">
         <v>0.62999999523162842</v>
       </c>
     </row>
@@ -4265,22 +4299,22 @@
       <c r="AB37">
         <v>2</v>
       </c>
-      <c r="AC37">
+      <c r="AC37" s="1">
         <v>0.43999999761581421</v>
       </c>
-      <c r="AD37">
+      <c r="AD37" s="1">
         <v>2.5099999904632568</v>
       </c>
-      <c r="AE37">
+      <c r="AE37" s="1">
         <v>2.119999885559082</v>
       </c>
-      <c r="AF37">
+      <c r="AF37" s="1">
         <v>0.92000001668930054</v>
       </c>
-      <c r="AG37">
+      <c r="AG37" s="1">
         <v>0.77999997138977051</v>
       </c>
-      <c r="AH37">
+      <c r="AH37" s="1">
         <v>1.1799999475479126</v>
       </c>
     </row>
@@ -4369,22 +4403,22 @@
       <c r="AB38">
         <v>1</v>
       </c>
-      <c r="AC38">
+      <c r="AC38" s="1">
         <v>0.76999998092651367</v>
       </c>
-      <c r="AD38">
+      <c r="AD38" s="1">
         <v>0.49000000953674316</v>
       </c>
-      <c r="AE38">
+      <c r="AE38" s="1">
         <v>0.30000001192092896</v>
       </c>
-      <c r="AF38">
+      <c r="AF38" s="1">
         <v>0.76999998092651367</v>
       </c>
-      <c r="AG38">
+      <c r="AG38" s="1">
         <v>0.97000002861022949</v>
       </c>
-      <c r="AH38">
+      <c r="AH38" s="1">
         <v>0.87000000476837158</v>
       </c>
     </row>
@@ -4473,22 +4507,22 @@
       <c r="AB39">
         <v>2</v>
       </c>
-      <c r="AC39">
+      <c r="AC39" s="1">
         <v>0.30000001192092896</v>
       </c>
-      <c r="AD39">
+      <c r="AD39" s="1">
         <v>1.0099999904632568</v>
       </c>
-      <c r="AE39">
+      <c r="AE39" s="1">
         <v>0.77999997138977051</v>
       </c>
-      <c r="AF39">
+      <c r="AF39" s="1">
         <v>0.72000002861022949</v>
       </c>
-      <c r="AG39">
+      <c r="AG39" s="1">
         <v>0.63999998569488525</v>
       </c>
-      <c r="AH39">
+      <c r="AH39" s="1">
         <v>0.68999999761581421</v>
       </c>
     </row>
@@ -4577,22 +4611,22 @@
       <c r="AB40">
         <v>1</v>
       </c>
-      <c r="AC40">
+      <c r="AC40" s="1">
         <v>0.5</v>
       </c>
-      <c r="AD40">
+      <c r="AD40" s="1">
         <v>1.1399999856948853</v>
       </c>
-      <c r="AE40">
+      <c r="AE40" s="1">
         <v>0.28999999165534973</v>
       </c>
-      <c r="AF40">
+      <c r="AF40" s="1">
         <v>0.67000001668930054</v>
       </c>
-      <c r="AG40">
+      <c r="AG40" s="1">
         <v>1.0499999523162842</v>
       </c>
-      <c r="AH40">
+      <c r="AH40" s="1">
         <v>0.56000000238418579</v>
       </c>
     </row>
@@ -4681,22 +4715,22 @@
       <c r="AB41">
         <v>2</v>
       </c>
-      <c r="AC41">
+      <c r="AC41" s="1">
         <v>0.40999999642372131</v>
       </c>
-      <c r="AD41">
+      <c r="AD41" s="1">
         <v>1.8799999952316284</v>
       </c>
-      <c r="AE41">
+      <c r="AE41" s="1">
         <v>0.6600000262260437</v>
       </c>
-      <c r="AF41">
+      <c r="AF41" s="1">
         <v>0.81999999284744263</v>
       </c>
-      <c r="AG41">
+      <c r="AG41" s="1">
         <v>1.6299999952316284</v>
       </c>
-      <c r="AH41">
+      <c r="AH41" s="1">
         <v>0.61000001430511475</v>
       </c>
     </row>
@@ -4785,16 +4819,16 @@
       <c r="AB42">
         <v>1</v>
       </c>
-      <c r="AC42">
+      <c r="AC42" s="1">
         <v>1.5199999809265137</v>
       </c>
-      <c r="AE42">
+      <c r="AE42" s="1">
         <v>0.33000001311302185</v>
       </c>
-      <c r="AF42">
+      <c r="AF42" s="1">
         <v>1.0199999809265137</v>
       </c>
-      <c r="AH42">
+      <c r="AH42" s="1">
         <v>0.76999998092651367</v>
       </c>
     </row>
@@ -4883,22 +4917,22 @@
       <c r="AB43">
         <v>2</v>
       </c>
-      <c r="AC43">
+      <c r="AC43" s="1">
         <v>0.34000000357627869</v>
       </c>
-      <c r="AD43">
+      <c r="AD43" s="1">
         <v>0.87999999523162842</v>
       </c>
-      <c r="AE43">
+      <c r="AE43" s="1">
         <v>1.0800000429153442</v>
       </c>
-      <c r="AF43">
+      <c r="AF43" s="1">
         <v>0.75</v>
       </c>
-      <c r="AG43">
+      <c r="AG43" s="1">
         <v>0.6600000262260437</v>
       </c>
-      <c r="AH43">
+      <c r="AH43" s="1">
         <v>1.5399999618530273</v>
       </c>
     </row>
@@ -4987,22 +5021,22 @@
       <c r="AB44">
         <v>1</v>
       </c>
-      <c r="AC44">
+      <c r="AC44" s="1">
         <v>0.50999999046325684</v>
       </c>
-      <c r="AD44">
+      <c r="AD44" s="1">
         <v>0.34000000357627869</v>
       </c>
-      <c r="AE44">
+      <c r="AE44" s="1">
         <v>0.33000001311302185</v>
       </c>
-      <c r="AF44">
+      <c r="AF44" s="1">
         <v>0.63999998569488525</v>
       </c>
-      <c r="AG44">
+      <c r="AG44" s="1">
         <v>0.8399999737739563</v>
       </c>
-      <c r="AH44">
+      <c r="AH44" s="1">
         <v>0.56000000238418579</v>
       </c>
     </row>
@@ -5091,22 +5125,22 @@
       <c r="AB45">
         <v>2</v>
       </c>
-      <c r="AC45">
+      <c r="AC45" s="1">
         <v>0.23000000417232513</v>
       </c>
-      <c r="AD45">
+      <c r="AD45" s="1">
         <v>1.0900000333786011</v>
       </c>
-      <c r="AE45">
+      <c r="AE45" s="1">
         <v>0.38999998569488525</v>
       </c>
-      <c r="AF45">
+      <c r="AF45" s="1">
         <v>0.6600000262260437</v>
       </c>
-      <c r="AG45">
+      <c r="AG45" s="1">
         <v>1.1100000143051147</v>
       </c>
-      <c r="AH45">
+      <c r="AH45" s="1">
         <v>0.81999999284744263</v>
       </c>
     </row>
@@ -5195,22 +5229,22 @@
       <c r="AB46">
         <v>1</v>
       </c>
-      <c r="AC46">
+      <c r="AC46" s="1">
         <v>0.92000001668930054</v>
       </c>
-      <c r="AD46">
+      <c r="AD46" s="1">
         <v>0.34000000357627869</v>
       </c>
-      <c r="AE46">
+      <c r="AE46" s="1">
         <v>0.23999999463558197</v>
       </c>
-      <c r="AF46">
+      <c r="AF46" s="1">
         <v>0.79000002145767212</v>
       </c>
-      <c r="AG46">
+      <c r="AG46" s="1">
         <v>0.75999999046325684</v>
       </c>
-      <c r="AH46">
+      <c r="AH46" s="1">
         <v>0.6600000262260437</v>
       </c>
     </row>
@@ -5299,22 +5333,22 @@
       <c r="AB47">
         <v>2</v>
       </c>
-      <c r="AC47">
+      <c r="AC47" s="1">
         <v>0.37999999523162842</v>
       </c>
-      <c r="AD47">
+      <c r="AD47" s="1">
         <v>1.7400000095367432</v>
       </c>
-      <c r="AE47">
+      <c r="AE47" s="1">
         <v>1.2799999713897705</v>
       </c>
-      <c r="AF47">
+      <c r="AF47" s="1">
         <v>1.059999942779541</v>
       </c>
-      <c r="AG47">
+      <c r="AG47" s="1">
         <v>1.6100000143051147</v>
       </c>
-      <c r="AH47">
+      <c r="AH47" s="1">
         <v>1.7999999523162842</v>
       </c>
     </row>
@@ -5403,22 +5437,22 @@
       <c r="AB48">
         <v>1</v>
       </c>
-      <c r="AC48">
+      <c r="AC48" s="1">
         <v>1.1699999570846558</v>
       </c>
-      <c r="AD48">
+      <c r="AD48" s="1">
         <v>1.5299999713897705</v>
       </c>
-      <c r="AE48">
+      <c r="AE48" s="1">
         <v>0.23000000417232513</v>
       </c>
-      <c r="AF48">
+      <c r="AF48" s="1">
         <v>0.86000001430511475</v>
       </c>
-      <c r="AG48">
+      <c r="AG48" s="1">
         <v>1.1100000143051147</v>
       </c>
-      <c r="AH48">
+      <c r="AH48" s="1">
         <v>0.63999998569488525</v>
       </c>
     </row>
@@ -5507,22 +5541,22 @@
       <c r="AB49">
         <v>2</v>
       </c>
-      <c r="AC49">
+      <c r="AC49" s="1">
         <v>0.31000000238418579</v>
       </c>
-      <c r="AD49">
+      <c r="AD49" s="1">
         <v>0.73000001907348633</v>
       </c>
-      <c r="AE49">
+      <c r="AE49" s="1">
         <v>0.93999999761581421</v>
       </c>
-      <c r="AF49">
+      <c r="AF49" s="1">
         <v>1.1100000143051147</v>
       </c>
-      <c r="AG49">
+      <c r="AG49" s="1">
         <v>1.1599999666213989</v>
       </c>
-      <c r="AH49">
+      <c r="AH49" s="1">
         <v>1.0099999904632568</v>
       </c>
     </row>
@@ -5611,16 +5645,16 @@
       <c r="AB50">
         <v>1</v>
       </c>
-      <c r="AC50">
+      <c r="AC50" s="1">
         <v>0.43000000715255737</v>
       </c>
-      <c r="AD50">
+      <c r="AD50" s="1">
         <v>0.57999998331069946</v>
       </c>
-      <c r="AF50">
+      <c r="AF50" s="1">
         <v>0.72000002861022949</v>
       </c>
-      <c r="AG50">
+      <c r="AG50" s="1">
         <v>1.6200000047683716</v>
       </c>
     </row>
@@ -5709,22 +5743,22 @@
       <c r="AB51">
         <v>2</v>
       </c>
-      <c r="AC51">
+      <c r="AC51" s="1">
         <v>0.28999999165534973</v>
       </c>
-      <c r="AD51">
+      <c r="AD51" s="1">
         <v>1.5</v>
       </c>
-      <c r="AE51">
+      <c r="AE51" s="1">
         <v>1.0099999904632568</v>
       </c>
-      <c r="AF51">
+      <c r="AF51" s="1">
         <v>3.4500000476837158</v>
       </c>
-      <c r="AG51">
+      <c r="AG51" s="1">
         <v>1.309999942779541</v>
       </c>
-      <c r="AH51">
+      <c r="AH51" s="1">
         <v>0.81999999284744263</v>
       </c>
     </row>
@@ -5813,16 +5847,16 @@
       <c r="AB52">
         <v>1</v>
       </c>
-      <c r="AC52">
+      <c r="AC52" s="1">
         <v>1.0299999713897705</v>
       </c>
-      <c r="AD52">
+      <c r="AD52" s="1">
         <v>0.75</v>
       </c>
-      <c r="AF52">
+      <c r="AF52" s="1">
         <v>1.3500000238418579</v>
       </c>
-      <c r="AG52">
+      <c r="AG52" s="1">
         <v>1.4600000381469727</v>
       </c>
     </row>
@@ -5911,16 +5945,16 @@
       <c r="AB53">
         <v>2</v>
       </c>
-      <c r="AC53">
+      <c r="AC53" s="1">
         <v>0.63999998569488525</v>
       </c>
-      <c r="AD53">
+      <c r="AD53" s="1">
         <v>1.3799999952316284</v>
       </c>
-      <c r="AF53">
+      <c r="AF53" s="1">
         <v>1.3799999952316284</v>
       </c>
-      <c r="AG53">
+      <c r="AG53" s="1">
         <v>1.1200000047683716</v>
       </c>
     </row>
@@ -6009,22 +6043,22 @@
       <c r="AB54">
         <v>1</v>
       </c>
-      <c r="AC54">
+      <c r="AC54" s="1">
         <v>1.3899999856948853</v>
       </c>
-      <c r="AD54">
+      <c r="AD54" s="1">
         <v>1.0399999618530273</v>
       </c>
-      <c r="AE54">
+      <c r="AE54" s="1">
         <v>0.34999999403953552</v>
       </c>
-      <c r="AF54">
+      <c r="AF54" s="1">
         <v>0.6600000262260437</v>
       </c>
-      <c r="AG54">
+      <c r="AG54" s="1">
         <v>1.1100000143051147</v>
       </c>
-      <c r="AH54">
+      <c r="AH54" s="1">
         <v>0.64999997615814209</v>
       </c>
     </row>
@@ -6113,22 +6147,22 @@
       <c r="AB55">
         <v>2</v>
       </c>
-      <c r="AC55">
+      <c r="AC55" s="1">
         <v>0.67000001668930054</v>
       </c>
-      <c r="AD55">
+      <c r="AD55" s="1">
         <v>0.17000000178813934</v>
       </c>
-      <c r="AE55">
+      <c r="AE55" s="1">
         <v>0.72000002861022949</v>
       </c>
-      <c r="AF55">
+      <c r="AF55" s="1">
         <v>0.76999998092651367</v>
       </c>
-      <c r="AG55">
+      <c r="AG55" s="1">
         <v>0.5899999737739563</v>
       </c>
-      <c r="AH55">
+      <c r="AH55" s="1">
         <v>0.61000001430511475</v>
       </c>
     </row>
@@ -6217,22 +6251,22 @@
       <c r="AB56">
         <v>1</v>
       </c>
-      <c r="AC56">
+      <c r="AC56" s="1">
         <v>1.7400000095367432</v>
       </c>
-      <c r="AD56">
+      <c r="AD56" s="1">
         <v>0.56999999284744263</v>
       </c>
-      <c r="AE56">
+      <c r="AE56" s="1">
         <v>0.27000001072883606</v>
       </c>
-      <c r="AF56">
+      <c r="AF56" s="1">
         <v>0.87999999523162842</v>
       </c>
-      <c r="AG56">
+      <c r="AG56" s="1">
         <v>0.99000000953674316</v>
       </c>
-      <c r="AH56">
+      <c r="AH56" s="1">
         <v>0.95999997854232788</v>
       </c>
     </row>
@@ -6321,22 +6355,22 @@
       <c r="AB57">
         <v>2</v>
       </c>
-      <c r="AC57">
+      <c r="AC57" s="1">
         <v>0.51999998092651367</v>
       </c>
-      <c r="AD57">
+      <c r="AD57" s="1">
         <v>1.8400000333786011</v>
       </c>
-      <c r="AE57">
+      <c r="AE57" s="1">
         <v>4.7800002098083496</v>
       </c>
-      <c r="AF57">
+      <c r="AF57" s="1">
         <v>0.63999998569488525</v>
       </c>
-      <c r="AG57">
-        <v>1</v>
-      </c>
-      <c r="AH57">
+      <c r="AG57" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH57" s="1">
         <v>0.98000001907348633</v>
       </c>
     </row>
@@ -6425,16 +6459,16 @@
       <c r="AB58">
         <v>1</v>
       </c>
-      <c r="AD58">
+      <c r="AD58" s="1">
         <v>2.2899999618530273</v>
       </c>
-      <c r="AE58">
+      <c r="AE58" s="1">
         <v>0.25</v>
       </c>
-      <c r="AG58">
+      <c r="AG58" s="1">
         <v>1.3999999761581421</v>
       </c>
-      <c r="AH58">
+      <c r="AH58" s="1">
         <v>0.75999999046325684</v>
       </c>
     </row>
@@ -6523,22 +6557,22 @@
       <c r="AB59">
         <v>2</v>
       </c>
-      <c r="AC59">
+      <c r="AC59" s="1">
         <v>1.440000057220459</v>
       </c>
-      <c r="AD59">
+      <c r="AD59" s="1">
         <v>0.69999998807907104</v>
       </c>
-      <c r="AE59">
+      <c r="AE59" s="1">
         <v>0.57999998331069946</v>
       </c>
-      <c r="AF59">
+      <c r="AF59" s="1">
         <v>1.2599999904632568</v>
       </c>
-      <c r="AG59">
+      <c r="AG59" s="1">
         <v>0.86000001430511475</v>
       </c>
-      <c r="AH59">
+      <c r="AH59" s="1">
         <v>0.81999999284744263</v>
       </c>
     </row>
@@ -6627,16 +6661,16 @@
       <c r="AB60">
         <v>1</v>
       </c>
-      <c r="AC60">
+      <c r="AC60" s="1">
         <v>2.0299999713897705</v>
       </c>
-      <c r="AD60">
+      <c r="AD60" s="1">
         <v>0.23999999463558197</v>
       </c>
-      <c r="AF60">
+      <c r="AF60" s="1">
         <v>1.9500000476837158</v>
       </c>
-      <c r="AG60">
+      <c r="AG60" s="1">
         <v>0.63999998569488525</v>
       </c>
     </row>
@@ -6725,22 +6759,22 @@
       <c r="AB61">
         <v>2</v>
       </c>
-      <c r="AC61">
+      <c r="AC61" s="1">
         <v>0.2800000011920929</v>
       </c>
-      <c r="AD61">
+      <c r="AD61" s="1">
         <v>1.1799999475479126</v>
       </c>
-      <c r="AE61">
+      <c r="AE61" s="1">
         <v>1.1000000238418579</v>
       </c>
-      <c r="AF61">
+      <c r="AF61" s="1">
         <v>0.68999999761581421</v>
       </c>
-      <c r="AG61">
+      <c r="AG61" s="1">
         <v>0.93999999761581421</v>
       </c>
-      <c r="AH61">
+      <c r="AH61" s="1">
         <v>0.57999998331069946</v>
       </c>
     </row>
@@ -6829,22 +6863,22 @@
       <c r="AB62">
         <v>1</v>
       </c>
-      <c r="AC62">
+      <c r="AC62" s="1">
         <v>0.23000000417232513</v>
       </c>
-      <c r="AD62">
+      <c r="AD62" s="1">
         <v>0.2800000011920929</v>
       </c>
-      <c r="AE62">
+      <c r="AE62" s="1">
         <v>0.2199999988079071</v>
       </c>
-      <c r="AF62">
+      <c r="AF62" s="1">
         <v>0.52999997138977051</v>
       </c>
-      <c r="AG62">
+      <c r="AG62" s="1">
         <v>0.67000001668930054</v>
       </c>
-      <c r="AH62">
+      <c r="AH62" s="1">
         <v>0.49000000953674316</v>
       </c>
     </row>
@@ -6933,22 +6967,22 @@
       <c r="AB63">
         <v>2</v>
       </c>
-      <c r="AC63">
+      <c r="AC63" s="1">
         <v>1.0700000524520874</v>
       </c>
-      <c r="AD63">
+      <c r="AD63" s="1">
         <v>1.5499999523162842</v>
       </c>
-      <c r="AE63">
+      <c r="AE63" s="1">
         <v>0.6600000262260437</v>
       </c>
-      <c r="AF63">
+      <c r="AF63" s="1">
         <v>0.87000000476837158</v>
       </c>
-      <c r="AG63">
+      <c r="AG63" s="1">
         <v>1.25</v>
       </c>
-      <c r="AH63">
+      <c r="AH63" s="1">
         <v>0.85000002384185791</v>
       </c>
     </row>
@@ -7037,22 +7071,22 @@
       <c r="AB64">
         <v>1</v>
       </c>
-      <c r="AC64">
+      <c r="AC64" s="1">
         <v>0.40000000596046448</v>
       </c>
-      <c r="AD64">
+      <c r="AD64" s="1">
         <v>0.51999998092651367</v>
       </c>
-      <c r="AE64">
+      <c r="AE64" s="1">
         <v>0.47999998927116394</v>
       </c>
-      <c r="AF64">
+      <c r="AF64" s="1">
         <v>0.55000001192092896</v>
       </c>
-      <c r="AG64">
+      <c r="AG64" s="1">
         <v>1.190000057220459</v>
       </c>
-      <c r="AH64">
+      <c r="AH64" s="1">
         <v>1.2899999618530273</v>
       </c>
     </row>
@@ -7141,16 +7175,16 @@
       <c r="AB65">
         <v>2</v>
       </c>
-      <c r="AC65">
+      <c r="AC65" s="1">
         <v>0.20999999344348907</v>
       </c>
-      <c r="AE65">
+      <c r="AE65" s="1">
         <v>0.50999999046325684</v>
       </c>
-      <c r="AF65">
+      <c r="AF65" s="1">
         <v>0.63999998569488525</v>
       </c>
-      <c r="AH65">
+      <c r="AH65" s="1">
         <v>0.5899999737739563</v>
       </c>
     </row>
@@ -7239,22 +7273,22 @@
       <c r="AB66">
         <v>1</v>
       </c>
-      <c r="AC66">
+      <c r="AC66" s="1">
         <v>1.4800000190734863</v>
       </c>
-      <c r="AD66">
+      <c r="AD66" s="1">
         <v>1.4199999570846558</v>
       </c>
-      <c r="AE66">
+      <c r="AE66" s="1">
         <v>0.10000000149011612</v>
       </c>
-      <c r="AF66">
+      <c r="AF66" s="1">
         <v>1.1699999570846558</v>
       </c>
-      <c r="AG66">
+      <c r="AG66" s="1">
         <v>1.0900000333786011</v>
       </c>
-      <c r="AH66">
+      <c r="AH66" s="1">
         <v>0.87000000476837158</v>
       </c>
     </row>
@@ -7343,22 +7377,22 @@
       <c r="AB67">
         <v>2</v>
       </c>
-      <c r="AC67">
+      <c r="AC67" s="1">
         <v>0.34000000357627869</v>
       </c>
-      <c r="AD67">
+      <c r="AD67" s="1">
         <v>0.50999999046325684</v>
       </c>
-      <c r="AE67">
+      <c r="AE67" s="1">
         <v>0.81000000238418579</v>
       </c>
-      <c r="AF67">
+      <c r="AF67" s="1">
         <v>0.61000001430511475</v>
       </c>
-      <c r="AG67">
+      <c r="AG67" s="1">
         <v>0.87000000476837158</v>
       </c>
-      <c r="AH67">
+      <c r="AH67" s="1">
         <v>0.81000000238418579</v>
       </c>
     </row>
@@ -7447,22 +7481,22 @@
       <c r="AB68">
         <v>1</v>
       </c>
-      <c r="AC68">
+      <c r="AC68" s="1">
         <v>1.4900000095367432</v>
       </c>
-      <c r="AD68">
+      <c r="AD68" s="1">
         <v>1.6799999475479126</v>
       </c>
-      <c r="AE68">
+      <c r="AE68" s="1">
         <v>0.18999999761581421</v>
       </c>
-      <c r="AF68">
+      <c r="AF68" s="1">
         <v>0.81999999284744263</v>
       </c>
-      <c r="AG68">
+      <c r="AG68" s="1">
         <v>1.2799999713897705</v>
       </c>
-      <c r="AH68">
+      <c r="AH68" s="1">
         <v>0.70999997854232788</v>
       </c>
     </row>
@@ -7551,22 +7585,22 @@
       <c r="AB69">
         <v>2</v>
       </c>
-      <c r="AC69">
+      <c r="AC69" s="1">
         <v>0.25</v>
       </c>
-      <c r="AD69">
+      <c r="AD69" s="1">
         <v>0.81000000238418579</v>
       </c>
-      <c r="AE69">
+      <c r="AE69" s="1">
         <v>0.77999997138977051</v>
       </c>
-      <c r="AF69">
+      <c r="AF69" s="1">
         <v>0.56999999284744263</v>
       </c>
-      <c r="AG69">
+      <c r="AG69" s="1">
         <v>1.0499999523162842</v>
       </c>
-      <c r="AH69">
+      <c r="AH69" s="1">
         <v>0.60000002384185791</v>
       </c>
     </row>
@@ -7655,22 +7689,22 @@
       <c r="AB70">
         <v>1</v>
       </c>
-      <c r="AC70">
+      <c r="AC70" s="1">
         <v>1.7899999618530273</v>
       </c>
-      <c r="AD70">
+      <c r="AD70" s="1">
         <v>0.99000000953674316</v>
       </c>
-      <c r="AE70">
+      <c r="AE70" s="1">
         <v>0.25999999046325684</v>
       </c>
-      <c r="AF70">
+      <c r="AF70" s="1">
         <v>1.6000000238418579</v>
       </c>
-      <c r="AG70">
+      <c r="AG70" s="1">
         <v>0.9100000262260437</v>
       </c>
-      <c r="AH70">
+      <c r="AH70" s="1">
         <v>0.76999998092651367</v>
       </c>
     </row>
@@ -7759,22 +7793,22 @@
       <c r="AB71">
         <v>2</v>
       </c>
-      <c r="AC71">
+      <c r="AC71" s="1">
         <v>0.28999999165534973</v>
       </c>
-      <c r="AD71">
+      <c r="AD71" s="1">
         <v>0.18000000715255737</v>
       </c>
-      <c r="AE71">
+      <c r="AE71" s="1">
         <v>1.9500000476837158</v>
       </c>
-      <c r="AF71">
+      <c r="AF71" s="1">
         <v>1.0299999713897705</v>
       </c>
-      <c r="AG71">
-        <v>1</v>
-      </c>
-      <c r="AH71">
+      <c r="AG71" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH71" s="1">
         <v>0.74000000953674316</v>
       </c>
     </row>
@@ -7863,16 +7897,16 @@
       <c r="AB72">
         <v>1</v>
       </c>
-      <c r="AC72">
+      <c r="AC72" s="1">
         <v>1.7699999809265137</v>
       </c>
-      <c r="AD72">
+      <c r="AD72" s="1">
         <v>0.37000000476837158</v>
       </c>
-      <c r="AF72">
+      <c r="AF72" s="1">
         <v>1.3200000524520874</v>
       </c>
-      <c r="AG72">
+      <c r="AG72" s="1">
         <v>0.82999998331069946</v>
       </c>
     </row>
@@ -7961,22 +7995,22 @@
       <c r="AB73">
         <v>2</v>
       </c>
-      <c r="AC73">
+      <c r="AC73" s="1">
         <v>1.809999942779541</v>
       </c>
-      <c r="AD73">
+      <c r="AD73" s="1">
         <v>1.1299999952316284</v>
       </c>
-      <c r="AE73">
+      <c r="AE73" s="1">
         <v>0.85000002384185791</v>
       </c>
-      <c r="AF73">
+      <c r="AF73" s="1">
         <v>1.0499999523162842</v>
       </c>
-      <c r="AG73">
+      <c r="AG73" s="1">
         <v>1.8799999952316284</v>
       </c>
-      <c r="AH73">
+      <c r="AH73" s="1">
         <v>0.85000002384185791</v>
       </c>
     </row>
@@ -8065,16 +8099,16 @@
       <c r="AB74">
         <v>1</v>
       </c>
-      <c r="AC74">
+      <c r="AC74" s="1">
         <v>1.4199999570846558</v>
       </c>
-      <c r="AD74">
+      <c r="AD74" s="1">
         <v>1.7200000286102295</v>
       </c>
-      <c r="AF74">
+      <c r="AF74" s="1">
         <v>1.2400000095367432</v>
       </c>
-      <c r="AG74">
+      <c r="AG74" s="1">
         <v>1.1599999666213989</v>
       </c>
     </row>
@@ -8163,22 +8197,22 @@
       <c r="AB75">
         <v>2</v>
       </c>
-      <c r="AC75">
+      <c r="AC75" s="1">
         <v>0.40000000596046448</v>
       </c>
-      <c r="AD75">
+      <c r="AD75" s="1">
         <v>1.75</v>
       </c>
-      <c r="AE75">
+      <c r="AE75" s="1">
         <v>1.0199999809265137</v>
       </c>
-      <c r="AF75">
+      <c r="AF75" s="1">
         <v>0.64999997615814209</v>
       </c>
-      <c r="AG75">
-        <v>1</v>
-      </c>
-      <c r="AH75">
+      <c r="AG75" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH75" s="1">
         <v>0.93000000715255737</v>
       </c>
     </row>
@@ -8267,16 +8301,16 @@
       <c r="AB76">
         <v>1</v>
       </c>
-      <c r="AD76">
+      <c r="AD76" s="1">
         <v>0.88999998569488525</v>
       </c>
-      <c r="AE76">
+      <c r="AE76" s="1">
         <v>0.25</v>
       </c>
-      <c r="AG76">
+      <c r="AG76" s="1">
         <v>0.97000002861022949</v>
       </c>
-      <c r="AH76">
+      <c r="AH76" s="1">
         <v>0.60000002384185791</v>
       </c>
     </row>
@@ -8365,22 +8399,22 @@
       <c r="AB77">
         <v>2</v>
       </c>
-      <c r="AC77">
+      <c r="AC77" s="1">
         <v>1.8500000238418579</v>
       </c>
-      <c r="AD77">
+      <c r="AD77" s="1">
         <v>2.1600000858306885</v>
       </c>
-      <c r="AE77">
+      <c r="AE77" s="1">
         <v>1.1200000047683716</v>
       </c>
-      <c r="AF77">
+      <c r="AF77" s="1">
         <v>1.2400000095367432</v>
       </c>
-      <c r="AG77">
+      <c r="AG77" s="1">
         <v>0.93000000715255737</v>
       </c>
-      <c r="AH77">
+      <c r="AH77" s="1">
         <v>1.0900000333786011</v>
       </c>
     </row>
@@ -8469,22 +8503,22 @@
       <c r="AB78">
         <v>1</v>
       </c>
-      <c r="AC78">
+      <c r="AC78" s="1">
         <v>2.4300000667572021</v>
       </c>
-      <c r="AD78">
+      <c r="AD78" s="1">
         <v>1.9900000095367432</v>
       </c>
-      <c r="AE78">
+      <c r="AE78" s="1">
         <v>0.56999999284744263</v>
       </c>
-      <c r="AF78">
+      <c r="AF78" s="1">
         <v>1.059999942779541</v>
       </c>
-      <c r="AG78">
+      <c r="AG78" s="1">
         <v>1.0399999618530273</v>
       </c>
-      <c r="AH78">
+      <c r="AH78" s="1">
         <v>0.87000000476837158</v>
       </c>
     </row>
@@ -8573,22 +8607,22 @@
       <c r="AB79">
         <v>2</v>
       </c>
-      <c r="AC79">
+      <c r="AC79" s="1">
         <v>1.5700000524520874</v>
       </c>
-      <c r="AD79">
+      <c r="AD79" s="1">
         <v>1.9500000476837158</v>
       </c>
-      <c r="AE79">
+      <c r="AE79" s="1">
         <v>0.9100000262260437</v>
       </c>
-      <c r="AF79">
+      <c r="AF79" s="1">
         <v>1.8500000238418579</v>
       </c>
-      <c r="AG79">
+      <c r="AG79" s="1">
         <v>1.5900000333786011</v>
       </c>
-      <c r="AH79">
+      <c r="AH79" s="1">
         <v>0.92000001668930054</v>
       </c>
     </row>
@@ -8677,22 +8711,22 @@
       <c r="AB80">
         <v>1</v>
       </c>
-      <c r="AC80">
+      <c r="AC80" s="1">
         <v>2.3199999332427979</v>
       </c>
-      <c r="AD80">
+      <c r="AD80" s="1">
         <v>0.99000000953674316</v>
       </c>
-      <c r="AE80">
+      <c r="AE80" s="1">
         <v>0.15000000596046448</v>
       </c>
-      <c r="AF80">
+      <c r="AF80" s="1">
         <v>1.2599999904632568</v>
       </c>
-      <c r="AG80">
+      <c r="AG80" s="1">
         <v>1.2899999618530273</v>
       </c>
-      <c r="AH80">
+      <c r="AH80" s="1">
         <v>0.94999998807907104</v>
       </c>
     </row>
@@ -8781,22 +8815,22 @@
       <c r="AB81">
         <v>2</v>
       </c>
-      <c r="AC81">
+      <c r="AC81" s="1">
         <v>0.25</v>
       </c>
-      <c r="AD81">
+      <c r="AD81" s="1">
         <v>0.75999999046325684</v>
       </c>
-      <c r="AE81">
+      <c r="AE81" s="1">
         <v>0.68999999761581421</v>
       </c>
-      <c r="AF81">
+      <c r="AF81" s="1">
         <v>0.64999997615814209</v>
       </c>
-      <c r="AG81">
+      <c r="AG81" s="1">
         <v>0.87999999523162842</v>
       </c>
-      <c r="AH81">
+      <c r="AH81" s="1">
         <v>0.56999999284744263</v>
       </c>
     </row>
@@ -8885,16 +8919,16 @@
       <c r="AB82">
         <v>1</v>
       </c>
-      <c r="AC82">
+      <c r="AC82" s="1">
         <v>1.3600000143051147</v>
       </c>
-      <c r="AD82">
+      <c r="AD82" s="1">
         <v>1.6200000047683716</v>
       </c>
-      <c r="AF82">
+      <c r="AF82" s="1">
         <v>1.1100000143051147</v>
       </c>
-      <c r="AG82">
+      <c r="AG82" s="1">
         <v>0.99000000953674316</v>
       </c>
     </row>
@@ -8983,16 +9017,16 @@
       <c r="AB83">
         <v>2</v>
       </c>
-      <c r="AC83">
+      <c r="AC83" s="1">
         <v>0.33000001311302185</v>
       </c>
-      <c r="AE83">
+      <c r="AE83" s="1">
         <v>0.57999998331069946</v>
       </c>
-      <c r="AF83">
+      <c r="AF83" s="1">
         <v>0.82999998331069946</v>
       </c>
-      <c r="AH83">
+      <c r="AH83" s="1">
         <v>0.63999998569488525</v>
       </c>
     </row>
@@ -9081,16 +9115,16 @@
       <c r="AB84">
         <v>1</v>
       </c>
-      <c r="AC84">
+      <c r="AC84" s="1">
         <v>0.20000000298023224</v>
       </c>
-      <c r="AD84">
+      <c r="AD84" s="1">
         <v>0.37999999523162842</v>
       </c>
-      <c r="AF84">
+      <c r="AF84" s="1">
         <v>0.69999998807907104</v>
       </c>
-      <c r="AG84">
+      <c r="AG84" s="1">
         <v>1.1499999761581421</v>
       </c>
     </row>
@@ -9179,22 +9213,22 @@
       <c r="AB85">
         <v>2</v>
       </c>
-      <c r="AC85">
+      <c r="AC85" s="1">
         <v>1.2400000095367432</v>
       </c>
-      <c r="AD85">
+      <c r="AD85" s="1">
         <v>1.559999942779541</v>
       </c>
-      <c r="AE85">
+      <c r="AE85" s="1">
         <v>0.64999997615814209</v>
       </c>
-      <c r="AF85">
+      <c r="AF85" s="1">
         <v>0.80000001192092896</v>
       </c>
-      <c r="AG85">
+      <c r="AG85" s="1">
         <v>0.89999997615814209</v>
       </c>
-      <c r="AH85">
+      <c r="AH85" s="1">
         <v>1.0099999904632568</v>
       </c>
     </row>
@@ -9283,16 +9317,16 @@
       <c r="AB86">
         <v>1</v>
       </c>
-      <c r="AC86">
+      <c r="AC86" s="1">
         <v>1.7200000286102295</v>
       </c>
-      <c r="AD86">
+      <c r="AD86" s="1">
         <v>0.20999999344348907</v>
       </c>
-      <c r="AF86">
+      <c r="AF86" s="1">
         <v>1.0800000429153442</v>
       </c>
-      <c r="AG86">
+      <c r="AG86" s="1">
         <v>0.62000000476837158</v>
       </c>
     </row>
@@ -9381,22 +9415,22 @@
       <c r="AB87">
         <v>2</v>
       </c>
-      <c r="AC87">
+      <c r="AC87" s="1">
         <v>1.7300000190734863</v>
       </c>
-      <c r="AD87">
+      <c r="AD87" s="1">
         <v>1.2699999809265137</v>
       </c>
-      <c r="AE87">
+      <c r="AE87" s="1">
         <v>3.0499999523162842</v>
       </c>
-      <c r="AF87">
+      <c r="AF87" s="1">
         <v>0.89999997615814209</v>
       </c>
-      <c r="AG87">
+      <c r="AG87" s="1">
         <v>1.6799999475479126</v>
       </c>
-      <c r="AH87">
+      <c r="AH87" s="1">
         <v>1.0199999809265137</v>
       </c>
     </row>
@@ -9485,16 +9519,16 @@
       <c r="AB88">
         <v>1</v>
       </c>
-      <c r="AC88">
+      <c r="AC88" s="1">
         <v>1.4299999475479126</v>
       </c>
-      <c r="AD88">
+      <c r="AD88" s="1">
         <v>1.309999942779541</v>
       </c>
-      <c r="AF88">
+      <c r="AF88" s="1">
         <v>0.97000002861022949</v>
       </c>
-      <c r="AG88">
+      <c r="AG88" s="1">
         <v>1.4700000286102295</v>
       </c>
     </row>
@@ -9583,22 +9617,22 @@
       <c r="AB89">
         <v>2</v>
       </c>
-      <c r="AC89">
+      <c r="AC89" s="1">
         <v>0.36000001430511475</v>
       </c>
-      <c r="AD89">
+      <c r="AD89" s="1">
         <v>1.7400000095367432</v>
       </c>
-      <c r="AE89">
+      <c r="AE89" s="1">
         <v>0.97000002861022949</v>
       </c>
-      <c r="AF89">
+      <c r="AF89" s="1">
         <v>0.72000002861022949</v>
       </c>
-      <c r="AG89">
+      <c r="AG89" s="1">
         <v>1.3300000429153442</v>
       </c>
-      <c r="AH89">
+      <c r="AH89" s="1">
         <v>1.0900000333786011</v>
       </c>
     </row>
@@ -9687,16 +9721,16 @@
       <c r="AB90">
         <v>1</v>
       </c>
-      <c r="AC90">
+      <c r="AC90" s="1">
         <v>0.28999999165534973</v>
       </c>
-      <c r="AD90">
+      <c r="AD90" s="1">
         <v>0.44999998807907104</v>
       </c>
-      <c r="AF90">
+      <c r="AF90" s="1">
         <v>0.76999998092651367</v>
       </c>
-      <c r="AG90">
+      <c r="AG90" s="1">
         <v>1.1299999952316284</v>
       </c>
     </row>
@@ -9785,22 +9819,22 @@
       <c r="AB91">
         <v>2</v>
       </c>
-      <c r="AC91">
+      <c r="AC91" s="1">
         <v>0.80000001192092896</v>
       </c>
-      <c r="AD91">
+      <c r="AD91" s="1">
         <v>1.75</v>
       </c>
-      <c r="AE91">
+      <c r="AE91" s="1">
         <v>1.8200000524520874</v>
       </c>
-      <c r="AF91">
+      <c r="AF91" s="1">
         <v>0.87000000476837158</v>
       </c>
-      <c r="AG91">
+      <c r="AG91" s="1">
         <v>1.0499999523162842</v>
       </c>
-      <c r="AH91">
+      <c r="AH91" s="1">
         <v>0.97000002861022949</v>
       </c>
     </row>
@@ -9889,16 +9923,16 @@
       <c r="AB92">
         <v>1</v>
       </c>
-      <c r="AC92">
+      <c r="AC92" s="1">
         <v>0.69999998807907104</v>
       </c>
-      <c r="AD92">
+      <c r="AD92" s="1">
         <v>1.7200000286102295</v>
       </c>
-      <c r="AF92">
+      <c r="AF92" s="1">
         <v>1.0099999904632568</v>
       </c>
-      <c r="AG92">
+      <c r="AG92" s="1">
         <v>1.4900000095367432</v>
       </c>
     </row>
@@ -9987,22 +10021,22 @@
       <c r="AB93">
         <v>2</v>
       </c>
-      <c r="AC93">
+      <c r="AC93" s="1">
         <v>0.25</v>
       </c>
-      <c r="AD93">
+      <c r="AD93" s="1">
         <v>1.4600000381469727</v>
       </c>
-      <c r="AE93">
+      <c r="AE93" s="1">
         <v>0.64999997615814209</v>
       </c>
-      <c r="AF93">
+      <c r="AF93" s="1">
         <v>0.64999997615814209</v>
       </c>
-      <c r="AG93">
+      <c r="AG93" s="1">
         <v>1.4299999475479126</v>
       </c>
-      <c r="AH93">
+      <c r="AH93" s="1">
         <v>0.56999999284744263</v>
       </c>
     </row>
@@ -10091,22 +10125,22 @@
       <c r="AB94">
         <v>2</v>
       </c>
-      <c r="AC94">
+      <c r="AC94" s="1">
         <v>0.56000000238418579</v>
       </c>
-      <c r="AD94">
+      <c r="AD94" s="1">
         <v>0.5</v>
       </c>
-      <c r="AE94">
+      <c r="AE94" s="1">
         <v>0.62999999523162842</v>
       </c>
-      <c r="AF94">
+      <c r="AF94" s="1">
         <v>1.0299999713897705</v>
       </c>
-      <c r="AG94">
+      <c r="AG94" s="1">
         <v>1.5099999904632568</v>
       </c>
-      <c r="AH94">
+      <c r="AH94" s="1">
         <v>0.74000000953674316</v>
       </c>
     </row>
@@ -10195,16 +10229,16 @@
       <c r="AB95">
         <v>1</v>
       </c>
-      <c r="AC95">
+      <c r="AC95" s="1">
         <v>1.5</v>
       </c>
-      <c r="AD95">
+      <c r="AD95" s="1">
         <v>1.2599999904632568</v>
       </c>
-      <c r="AF95">
+      <c r="AF95" s="1">
         <v>1.190000057220459</v>
       </c>
-      <c r="AG95">
+      <c r="AG95" s="1">
         <v>1.25</v>
       </c>
     </row>
@@ -10293,22 +10327,22 @@
       <c r="AB96">
         <v>2</v>
       </c>
-      <c r="AC96">
+      <c r="AC96" s="1">
         <v>1.6000000238418579</v>
       </c>
-      <c r="AD96">
+      <c r="AD96" s="1">
         <v>0.89999997615814209</v>
       </c>
-      <c r="AE96">
+      <c r="AE96" s="1">
         <v>0.88999998569488525</v>
       </c>
-      <c r="AF96">
+      <c r="AF96" s="1">
         <v>0.97000002861022949</v>
       </c>
-      <c r="AG96">
+      <c r="AG96" s="1">
         <v>1.1599999666213989</v>
       </c>
-      <c r="AH96">
+      <c r="AH96" s="1">
         <v>1</v>
       </c>
     </row>
@@ -10397,22 +10431,22 @@
       <c r="AB97">
         <v>1</v>
       </c>
-      <c r="AC97">
+      <c r="AC97" s="1">
         <v>0.5</v>
       </c>
-      <c r="AD97">
+      <c r="AD97" s="1">
         <v>0.51999998092651367</v>
       </c>
-      <c r="AE97">
+      <c r="AE97" s="1">
         <v>0.5</v>
       </c>
-      <c r="AF97">
+      <c r="AF97" s="1">
         <v>0.75</v>
       </c>
-      <c r="AG97">
+      <c r="AG97" s="1">
         <v>1.0099999904632568</v>
       </c>
-      <c r="AH97">
+      <c r="AH97" s="1">
         <v>0.70999997854232788</v>
       </c>
     </row>
@@ -10501,22 +10535,22 @@
       <c r="AB98">
         <v>2</v>
       </c>
-      <c r="AC98">
+      <c r="AC98" s="1">
         <v>0.23000000417232513</v>
       </c>
-      <c r="AD98">
+      <c r="AD98" s="1">
         <v>3.0999999046325684</v>
       </c>
-      <c r="AE98">
+      <c r="AE98" s="1">
         <v>0.43000000715255737</v>
       </c>
-      <c r="AF98">
+      <c r="AF98" s="1">
         <v>0.62000000476837158</v>
       </c>
-      <c r="AG98">
+      <c r="AG98" s="1">
         <v>1.4700000286102295</v>
       </c>
-      <c r="AH98">
+      <c r="AH98" s="1">
         <v>0.5899999737739563</v>
       </c>
     </row>
@@ -10605,22 +10639,22 @@
       <c r="AB99">
         <v>1</v>
       </c>
-      <c r="AC99">
+      <c r="AC99" s="1">
         <v>0.68000000715255737</v>
       </c>
-      <c r="AD99">
+      <c r="AD99" s="1">
         <v>0.31999999284744263</v>
       </c>
-      <c r="AE99">
+      <c r="AE99" s="1">
         <v>0.38999998569488525</v>
       </c>
-      <c r="AF99">
+      <c r="AF99" s="1">
         <v>0.87999999523162842</v>
       </c>
-      <c r="AG99">
+      <c r="AG99" s="1">
         <v>0.56000000238418579</v>
       </c>
-      <c r="AH99">
+      <c r="AH99" s="1">
         <v>0.57999998331069946</v>
       </c>
     </row>
@@ -10709,22 +10743,22 @@
       <c r="AB100">
         <v>2</v>
       </c>
-      <c r="AC100">
+      <c r="AC100" s="1">
         <v>0.85000002384185791</v>
       </c>
-      <c r="AD100">
+      <c r="AD100" s="1">
         <v>0.92000001668930054</v>
       </c>
-      <c r="AE100">
+      <c r="AE100" s="1">
         <v>0.68000000715255737</v>
       </c>
-      <c r="AF100">
+      <c r="AF100" s="1">
         <v>0.95999997854232788</v>
       </c>
-      <c r="AG100">
+      <c r="AG100" s="1">
         <v>1.1399999856948853</v>
       </c>
-      <c r="AH100">
+      <c r="AH100" s="1">
         <v>1.1299999952316284</v>
       </c>
     </row>
@@ -10813,16 +10847,16 @@
       <c r="AB101">
         <v>1</v>
       </c>
-      <c r="AC101">
+      <c r="AC101" s="1">
         <v>2.2100000381469727</v>
       </c>
-      <c r="AD101">
+      <c r="AD101" s="1">
         <v>1.059999942779541</v>
       </c>
-      <c r="AF101">
+      <c r="AF101" s="1">
         <v>2.059999942779541</v>
       </c>
-      <c r="AG101">
+      <c r="AG101" s="1">
         <v>0.99000000953674316</v>
       </c>
     </row>
@@ -10911,22 +10945,22 @@
       <c r="AB102">
         <v>2</v>
       </c>
-      <c r="AC102">
+      <c r="AC102" s="1">
         <v>2.4800000190734863</v>
       </c>
-      <c r="AD102">
+      <c r="AD102" s="1">
         <v>1.5800000429153442</v>
       </c>
-      <c r="AE102">
+      <c r="AE102" s="1">
         <v>2.0899999141693115</v>
       </c>
-      <c r="AF102">
+      <c r="AF102" s="1">
         <v>0.94999998807907104</v>
       </c>
-      <c r="AG102">
+      <c r="AG102" s="1">
         <v>1.1000000238418579</v>
       </c>
-      <c r="AH102">
+      <c r="AH102" s="1">
         <v>1.0299999713897705</v>
       </c>
     </row>
@@ -11015,22 +11049,22 @@
       <c r="AB103">
         <v>1</v>
       </c>
-      <c r="AC103">
+      <c r="AC103" s="1">
         <v>1.8799999952316284</v>
       </c>
-      <c r="AD103">
+      <c r="AD103" s="1">
         <v>1.4299999475479126</v>
       </c>
-      <c r="AE103">
+      <c r="AE103" s="1">
         <v>0.20999999344348907</v>
       </c>
-      <c r="AF103">
+      <c r="AF103" s="1">
         <v>0.92000001668930054</v>
       </c>
-      <c r="AG103">
+      <c r="AG103" s="1">
         <v>1.0900000333786011</v>
       </c>
-      <c r="AH103">
+      <c r="AH103" s="1">
         <v>0.6600000262260437</v>
       </c>
     </row>
@@ -11119,22 +11153,22 @@
       <c r="AB104">
         <v>2</v>
       </c>
-      <c r="AC104">
+      <c r="AC104" s="1">
         <v>1.5199999809265137</v>
       </c>
-      <c r="AD104">
+      <c r="AD104" s="1">
         <v>1.4099999666213989</v>
       </c>
-      <c r="AE104">
+      <c r="AE104" s="1">
         <v>0.75</v>
       </c>
-      <c r="AF104">
+      <c r="AF104" s="1">
         <v>1.0700000524520874</v>
       </c>
-      <c r="AG104">
+      <c r="AG104" s="1">
         <v>1.0199999809265137</v>
       </c>
-      <c r="AH104">
+      <c r="AH104" s="1">
         <v>0.73000001907348633</v>
       </c>
     </row>
@@ -11223,22 +11257,22 @@
       <c r="AB105">
         <v>1</v>
       </c>
-      <c r="AC105">
+      <c r="AC105" s="1">
         <v>0.63999998569488525</v>
       </c>
-      <c r="AD105">
+      <c r="AD105" s="1">
         <v>1.7400000095367432</v>
       </c>
-      <c r="AE105">
+      <c r="AE105" s="1">
         <v>0.82999998331069946</v>
       </c>
-      <c r="AF105">
+      <c r="AF105" s="1">
         <v>0.74000000953674316</v>
       </c>
-      <c r="AG105">
+      <c r="AG105" s="1">
         <v>1.690000057220459</v>
       </c>
-      <c r="AH105">
+      <c r="AH105" s="1">
         <v>0.50999999046325684</v>
       </c>
     </row>
@@ -11327,22 +11361,22 @@
       <c r="AB106">
         <v>2</v>
       </c>
-      <c r="AC106">
+      <c r="AC106" s="1">
         <v>1.0199999809265137</v>
       </c>
-      <c r="AD106">
+      <c r="AD106" s="1">
         <v>0.88999998569488525</v>
       </c>
-      <c r="AE106">
+      <c r="AE106" s="1">
         <v>0.46000000834465027</v>
       </c>
-      <c r="AF106">
+      <c r="AF106" s="1">
         <v>1.0199999809265137</v>
       </c>
-      <c r="AG106">
+      <c r="AG106" s="1">
         <v>1.4099999666213989</v>
       </c>
-      <c r="AH106">
+      <c r="AH106" s="1">
         <v>0.73000001907348633</v>
       </c>
     </row>
@@ -11431,22 +11465,22 @@
       <c r="AB107">
         <v>1</v>
       </c>
-      <c r="AC107">
+      <c r="AC107" s="1">
         <v>1.2400000095367432</v>
       </c>
-      <c r="AD107">
+      <c r="AD107" s="1">
         <v>1.2799999713897705</v>
       </c>
-      <c r="AE107">
+      <c r="AE107" s="1">
         <v>0.37000000476837158</v>
       </c>
-      <c r="AF107">
+      <c r="AF107" s="1">
         <v>1.9700000286102295</v>
       </c>
-      <c r="AG107">
+      <c r="AG107" s="1">
         <v>1.1799999475479126</v>
       </c>
-      <c r="AH107">
+      <c r="AH107" s="1">
         <v>0.80000001192092896</v>
       </c>
     </row>
@@ -11535,22 +11569,22 @@
       <c r="AB108">
         <v>2</v>
       </c>
-      <c r="AC108">
+      <c r="AC108" s="1">
         <v>0.37000000476837158</v>
       </c>
-      <c r="AD108">
+      <c r="AD108" s="1">
         <v>1.3999999761581421</v>
       </c>
-      <c r="AE108">
+      <c r="AE108" s="1">
         <v>1.4700000286102295</v>
       </c>
-      <c r="AF108">
+      <c r="AF108" s="1">
         <v>1.0299999713897705</v>
       </c>
-      <c r="AG108">
+      <c r="AG108" s="1">
         <v>0.93999999761581421</v>
       </c>
-      <c r="AH108">
+      <c r="AH108" s="1">
         <v>0.89999997615814209</v>
       </c>
     </row>
@@ -11639,22 +11673,22 @@
       <c r="AB109">
         <v>1</v>
       </c>
-      <c r="AC109">
+      <c r="AC109" s="1">
         <v>2.6500000953674316</v>
       </c>
-      <c r="AD109">
+      <c r="AD109" s="1">
         <v>0.54000002145767212</v>
       </c>
-      <c r="AE109">
+      <c r="AE109" s="1">
         <v>0.56000000238418579</v>
       </c>
-      <c r="AF109">
+      <c r="AF109" s="1">
         <v>2.2599999904632568</v>
       </c>
-      <c r="AG109">
+      <c r="AG109" s="1">
         <v>1.0700000524520874</v>
       </c>
-      <c r="AH109">
+      <c r="AH109" s="1">
         <v>0.69999998807907104</v>
       </c>
     </row>
@@ -11743,22 +11777,22 @@
       <c r="AB110">
         <v>2</v>
       </c>
-      <c r="AC110">
+      <c r="AC110" s="1">
         <v>2.2000000476837158</v>
       </c>
-      <c r="AD110">
+      <c r="AD110" s="1">
         <v>2.1800000667572021</v>
       </c>
-      <c r="AE110">
+      <c r="AE110" s="1">
         <v>1.3400000333786011</v>
       </c>
-      <c r="AF110">
+      <c r="AF110" s="1">
         <v>1.0399999618530273</v>
       </c>
-      <c r="AG110">
+      <c r="AG110" s="1">
         <v>1.2999999523162842</v>
       </c>
-      <c r="AH110">
+      <c r="AH110" s="1">
         <v>1.559999942779541</v>
       </c>
     </row>
@@ -11847,16 +11881,16 @@
       <c r="AB111">
         <v>1</v>
       </c>
-      <c r="AD111">
+      <c r="AD111" s="1">
         <v>1.4900000095367432</v>
       </c>
-      <c r="AE111">
+      <c r="AE111" s="1">
         <v>7.0000000298023224E-2</v>
       </c>
-      <c r="AG111">
+      <c r="AG111" s="1">
         <v>1.2599999904632568</v>
       </c>
-      <c r="AH111">
+      <c r="AH111" s="1">
         <v>0.68999999761581421</v>
       </c>
     </row>
@@ -11945,22 +11979,22 @@
       <c r="AB112">
         <v>2</v>
       </c>
-      <c r="AC112">
+      <c r="AC112" s="1">
         <v>1.8700000047683716</v>
       </c>
-      <c r="AD112">
+      <c r="AD112" s="1">
         <v>2.0399999618530273</v>
       </c>
-      <c r="AE112">
+      <c r="AE112" s="1">
         <v>0.88999998569488525</v>
       </c>
-      <c r="AF112">
+      <c r="AF112" s="1">
         <v>0.85000002384185791</v>
       </c>
-      <c r="AG112">
+      <c r="AG112" s="1">
         <v>1.1399999856948853</v>
       </c>
-      <c r="AH112">
+      <c r="AH112" s="1">
         <v>0.81999999284744263</v>
       </c>
     </row>
@@ -12049,22 +12083,22 @@
       <c r="AB113">
         <v>1</v>
       </c>
-      <c r="AC113">
+      <c r="AC113" s="1">
         <v>5.9999998658895493E-2</v>
       </c>
-      <c r="AD113">
+      <c r="AD113" s="1">
         <v>1.0800000429153442</v>
       </c>
-      <c r="AE113">
+      <c r="AE113" s="1">
         <v>0.33000001311302185</v>
       </c>
-      <c r="AF113">
+      <c r="AF113" s="1">
         <v>0.79000002145767212</v>
       </c>
-      <c r="AG113">
+      <c r="AG113" s="1">
         <v>1.059999942779541</v>
       </c>
-      <c r="AH113">
+      <c r="AH113" s="1">
         <v>1.3899999856948853</v>
       </c>
     </row>
@@ -12153,22 +12187,22 @@
       <c r="AB114">
         <v>2</v>
       </c>
-      <c r="AC114">
+      <c r="AC114" s="1">
         <v>1.0800000429153442</v>
       </c>
-      <c r="AD114">
+      <c r="AD114" s="1">
         <v>2.690000057220459</v>
       </c>
-      <c r="AE114">
+      <c r="AE114" s="1">
         <v>0.93999999761581421</v>
       </c>
-      <c r="AF114">
+      <c r="AF114" s="1">
         <v>0.95999997854232788</v>
       </c>
-      <c r="AG114">
+      <c r="AG114" s="1">
         <v>2.3299999237060547</v>
       </c>
-      <c r="AH114">
+      <c r="AH114" s="1">
         <v>0.8399999737739563</v>
       </c>
     </row>
@@ -12257,22 +12291,22 @@
       <c r="AB115">
         <v>1</v>
       </c>
-      <c r="AC115">
+      <c r="AC115" s="1">
         <v>0.33000001311302185</v>
       </c>
-      <c r="AD115">
+      <c r="AD115" s="1">
         <v>0.40000000596046448</v>
       </c>
-      <c r="AE115">
+      <c r="AE115" s="1">
         <v>0.33000001311302185</v>
       </c>
-      <c r="AF115">
+      <c r="AF115" s="1">
         <v>0.81999999284744263</v>
       </c>
-      <c r="AG115">
+      <c r="AG115" s="1">
         <v>0.73000001907348633</v>
       </c>
-      <c r="AH115">
+      <c r="AH115" s="1">
         <v>0.6600000262260437</v>
       </c>
     </row>
@@ -12361,22 +12395,22 @@
       <c r="AB116">
         <v>2</v>
       </c>
-      <c r="AC116">
+      <c r="AC116" s="1">
         <v>1.7400000095367432</v>
       </c>
-      <c r="AD116">
+      <c r="AD116" s="1">
         <v>0.97000002861022949</v>
       </c>
-      <c r="AE116">
+      <c r="AE116" s="1">
         <v>1.4199999570846558</v>
       </c>
-      <c r="AF116">
+      <c r="AF116" s="1">
         <v>1.0399999618530273</v>
       </c>
-      <c r="AG116">
+      <c r="AG116" s="1">
         <v>1.3799999952316284</v>
       </c>
-      <c r="AH116">
+      <c r="AH116" s="1">
         <v>0.92000001668930054</v>
       </c>
     </row>
@@ -12465,10 +12499,10 @@
       <c r="AB117">
         <v>1</v>
       </c>
-      <c r="AD117">
+      <c r="AD117" s="1">
         <v>0.49000000953674316</v>
       </c>
-      <c r="AG117">
+      <c r="AG117" s="1">
         <v>1.0700000524520874</v>
       </c>
     </row>
@@ -12557,22 +12591,22 @@
       <c r="AB118">
         <v>2</v>
       </c>
-      <c r="AC118">
+      <c r="AC118" s="1">
         <v>0.25999999046325684</v>
       </c>
-      <c r="AD118">
+      <c r="AD118" s="1">
         <v>0.56999999284744263</v>
       </c>
-      <c r="AE118">
+      <c r="AE118" s="1">
         <v>2.0799999237060547</v>
       </c>
-      <c r="AF118">
+      <c r="AF118" s="1">
         <v>0.56999999284744263</v>
       </c>
-      <c r="AG118">
+      <c r="AG118" s="1">
         <v>1.0700000524520874</v>
       </c>
-      <c r="AH118">
+      <c r="AH118" s="1">
         <v>0.60000002384185791</v>
       </c>
     </row>
@@ -12661,22 +12695,22 @@
       <c r="AB119">
         <v>1</v>
       </c>
-      <c r="AC119">
+      <c r="AC119" s="1">
         <v>0.77999997138977051</v>
       </c>
-      <c r="AD119">
+      <c r="AD119" s="1">
         <v>1.9700000286102295</v>
       </c>
-      <c r="AE119">
+      <c r="AE119" s="1">
         <v>5.000000074505806E-2</v>
       </c>
-      <c r="AF119">
+      <c r="AF119" s="1">
         <v>1.9600000381469727</v>
       </c>
-      <c r="AG119">
+      <c r="AG119" s="1">
         <v>0.99000000953674316</v>
       </c>
-      <c r="AH119">
+      <c r="AH119" s="1">
         <v>1.2200000286102295</v>
       </c>
     </row>
@@ -12765,22 +12799,22 @@
       <c r="AB120">
         <v>2</v>
       </c>
-      <c r="AC120">
+      <c r="AC120" s="1">
         <v>1.1000000238418579</v>
       </c>
-      <c r="AD120">
+      <c r="AD120" s="1">
         <v>0.70999997854232788</v>
       </c>
-      <c r="AE120">
+      <c r="AE120" s="1">
         <v>1.309999942779541</v>
       </c>
-      <c r="AF120">
+      <c r="AF120" s="1">
         <v>1.2000000476837158</v>
       </c>
-      <c r="AG120">
+      <c r="AG120" s="1">
         <v>0.87000000476837158</v>
       </c>
-      <c r="AH120">
+      <c r="AH120" s="1">
         <v>0.8399999737739563</v>
       </c>
     </row>
@@ -12869,22 +12903,22 @@
       <c r="AB121">
         <v>1</v>
       </c>
-      <c r="AC121">
+      <c r="AC121" s="1">
         <v>0.80000001192092896</v>
       </c>
-      <c r="AD121">
+      <c r="AD121" s="1">
         <v>0.10000000149011612</v>
       </c>
-      <c r="AE121">
+      <c r="AE121" s="1">
         <v>0.27000001072883606</v>
       </c>
-      <c r="AF121">
+      <c r="AF121" s="1">
         <v>0.64999997615814209</v>
       </c>
-      <c r="AG121">
+      <c r="AG121" s="1">
         <v>0.61000001430511475</v>
       </c>
-      <c r="AH121">
+      <c r="AH121" s="1">
         <v>0.5899999737739563</v>
       </c>
     </row>
@@ -12973,22 +13007,22 @@
       <c r="AB122">
         <v>2</v>
       </c>
-      <c r="AC122">
+      <c r="AC122" s="1">
         <v>0.20999999344348907</v>
       </c>
-      <c r="AD122">
+      <c r="AD122" s="1">
         <v>2.9000000953674316</v>
       </c>
-      <c r="AE122">
+      <c r="AE122" s="1">
         <v>0.6600000262260437</v>
       </c>
-      <c r="AF122">
+      <c r="AF122" s="1">
         <v>0.63999998569488525</v>
       </c>
-      <c r="AG122">
+      <c r="AG122" s="1">
         <v>1.8500000238418579</v>
       </c>
-      <c r="AH122">
+      <c r="AH122" s="1">
         <v>0.6600000262260437</v>
       </c>
     </row>
@@ -13077,16 +13111,16 @@
       <c r="AB123">
         <v>1</v>
       </c>
-      <c r="AC123">
+      <c r="AC123" s="1">
         <v>0.81000000238418579</v>
       </c>
-      <c r="AD123">
+      <c r="AD123" s="1">
         <v>0.54000002145767212</v>
       </c>
-      <c r="AF123">
+      <c r="AF123" s="1">
         <v>1.2300000190734863</v>
       </c>
-      <c r="AG123">
+      <c r="AG123" s="1">
         <v>1.0199999809265137</v>
       </c>
     </row>
@@ -13175,22 +13209,22 @@
       <c r="AB124">
         <v>2</v>
       </c>
-      <c r="AC124">
+      <c r="AC124" s="1">
         <v>0.68000000715255737</v>
       </c>
-      <c r="AD124">
+      <c r="AD124" s="1">
         <v>1.5800000429153442</v>
       </c>
-      <c r="AE124">
+      <c r="AE124" s="1">
         <v>1.2300000190734863</v>
       </c>
-      <c r="AF124">
+      <c r="AF124" s="1">
         <v>1.0700000524520874</v>
       </c>
-      <c r="AG124">
+      <c r="AG124" s="1">
         <v>1.3500000238418579</v>
       </c>
-      <c r="AH124">
+      <c r="AH124" s="1">
         <v>0.92000001668930054</v>
       </c>
     </row>
@@ -13279,22 +13313,22 @@
       <c r="AB125">
         <v>1</v>
       </c>
-      <c r="AC125">
+      <c r="AC125" s="1">
         <v>0.62999999523162842</v>
       </c>
-      <c r="AD125">
+      <c r="AD125" s="1">
         <v>0.63999998569488525</v>
       </c>
-      <c r="AE125">
+      <c r="AE125" s="1">
         <v>0.52999997138977051</v>
       </c>
-      <c r="AF125">
+      <c r="AF125" s="1">
         <v>0.92000001668930054</v>
       </c>
-      <c r="AG125">
+      <c r="AG125" s="1">
         <v>0.72000002861022949</v>
       </c>
-      <c r="AH125">
+      <c r="AH125" s="1">
         <v>0.77999997138977051</v>
       </c>
     </row>
@@ -13383,22 +13417,22 @@
       <c r="AB126">
         <v>2</v>
       </c>
-      <c r="AC126">
+      <c r="AC126" s="1">
         <v>0.86000001430511475</v>
       </c>
-      <c r="AD126">
+      <c r="AD126" s="1">
         <v>2.7799999713897705</v>
       </c>
-      <c r="AE126">
+      <c r="AE126" s="1">
         <v>1.0700000524520874</v>
       </c>
-      <c r="AF126">
+      <c r="AF126" s="1">
         <v>0.81000000238418579</v>
       </c>
-      <c r="AG126">
+      <c r="AG126" s="1">
         <v>1.3200000524520874</v>
       </c>
-      <c r="AH126">
+      <c r="AH126" s="1">
         <v>0.69999998807907104</v>
       </c>
     </row>
@@ -13487,22 +13521,22 @@
       <c r="AB127">
         <v>1</v>
       </c>
-      <c r="AC127">
+      <c r="AC127" s="1">
         <v>0.12999999523162842</v>
       </c>
-      <c r="AD127">
+      <c r="AD127" s="1">
         <v>0.34999999403953552</v>
       </c>
-      <c r="AE127">
+      <c r="AE127" s="1">
         <v>0.18999999761581421</v>
       </c>
-      <c r="AF127">
+      <c r="AF127" s="1">
         <v>0.64999997615814209</v>
       </c>
-      <c r="AG127">
+      <c r="AG127" s="1">
         <v>0.73000001907348633</v>
       </c>
-      <c r="AH127">
+      <c r="AH127" s="1">
         <v>0.56000000238418579</v>
       </c>
     </row>
@@ -13591,22 +13625,22 @@
       <c r="AB128">
         <v>2</v>
       </c>
-      <c r="AC128">
+      <c r="AC128" s="1">
         <v>0.40999999642372131</v>
       </c>
-      <c r="AD128">
+      <c r="AD128" s="1">
         <v>0.30000001192092896</v>
       </c>
-      <c r="AE128">
+      <c r="AE128" s="1">
         <v>0.60000002384185791</v>
       </c>
-      <c r="AF128">
+      <c r="AF128" s="1">
         <v>0.69999998807907104</v>
       </c>
-      <c r="AG128">
+      <c r="AG128" s="1">
         <v>0.80000001192092896</v>
       </c>
-      <c r="AH128">
+      <c r="AH128" s="1">
         <v>0.72000002861022949</v>
       </c>
     </row>
@@ -13695,16 +13729,16 @@
       <c r="AB129">
         <v>1</v>
       </c>
-      <c r="AC129">
+      <c r="AC129" s="1">
         <v>1.5800000429153442</v>
       </c>
-      <c r="AD129">
+      <c r="AD129" s="1">
         <v>0.88999998569488525</v>
       </c>
-      <c r="AF129">
+      <c r="AF129" s="1">
         <v>0.86000001430511475</v>
       </c>
-      <c r="AG129">
+      <c r="AG129" s="1">
         <v>1.2899999618530273</v>
       </c>
     </row>
@@ -13793,22 +13827,22 @@
       <c r="AB130">
         <v>2</v>
       </c>
-      <c r="AC130">
+      <c r="AC130" s="1">
         <v>0.18999999761581421</v>
       </c>
-      <c r="AD130">
+      <c r="AD130" s="1">
         <v>0.18000000715255737</v>
       </c>
-      <c r="AE130">
+      <c r="AE130" s="1">
         <v>0.51999998092651367</v>
       </c>
-      <c r="AF130">
+      <c r="AF130" s="1">
         <v>0.60000002384185791</v>
       </c>
-      <c r="AG130">
+      <c r="AG130" s="1">
         <v>0.55000001192092896</v>
       </c>
-      <c r="AH130">
+      <c r="AH130" s="1">
         <v>0.63999998569488525</v>
       </c>
     </row>
@@ -13897,16 +13931,16 @@
       <c r="AB131">
         <v>1</v>
       </c>
-      <c r="AD131">
+      <c r="AD131" s="1">
         <v>1.7699999809265137</v>
       </c>
-      <c r="AE131">
+      <c r="AE131" s="1">
         <v>0.33000001311302185</v>
       </c>
-      <c r="AG131">
+      <c r="AG131" s="1">
         <v>1.75</v>
       </c>
-      <c r="AH131">
+      <c r="AH131" s="1">
         <v>0.94999998807907104</v>
       </c>
     </row>
@@ -13995,22 +14029,22 @@
       <c r="AB132">
         <v>2</v>
       </c>
-      <c r="AC132">
+      <c r="AC132" s="1">
         <v>1.3799999952316284</v>
       </c>
-      <c r="AD132">
+      <c r="AD132" s="1">
         <v>1.0800000429153442</v>
       </c>
-      <c r="AE132">
+      <c r="AE132" s="1">
         <v>4.3600001335144043</v>
       </c>
-      <c r="AF132">
+      <c r="AF132" s="1">
         <v>1.1699999570846558</v>
       </c>
-      <c r="AG132">
+      <c r="AG132" s="1">
         <v>0.75</v>
       </c>
-      <c r="AH132">
+      <c r="AH132" s="1">
         <v>1.2699999809265137</v>
       </c>
     </row>
@@ -14099,22 +14133,22 @@
       <c r="AB133">
         <v>1</v>
       </c>
-      <c r="AC133">
+      <c r="AC133" s="1">
         <v>1.7899999618530273</v>
       </c>
-      <c r="AD133">
-        <v>1</v>
-      </c>
-      <c r="AE133">
+      <c r="AD133" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE133" s="1">
         <v>0.23999999463558197</v>
       </c>
-      <c r="AF133">
+      <c r="AF133" s="1">
         <v>0.79000002145767212</v>
       </c>
-      <c r="AG133">
+      <c r="AG133" s="1">
         <v>0.75</v>
       </c>
-      <c r="AH133">
+      <c r="AH133" s="1">
         <v>0.61000001430511475</v>
       </c>
     </row>
@@ -14203,22 +14237,22 @@
       <c r="AB134">
         <v>2</v>
       </c>
-      <c r="AC134">
+      <c r="AC134" s="1">
         <v>0.34999999403953552</v>
       </c>
-      <c r="AD134">
+      <c r="AD134" s="1">
         <v>0.70999997854232788</v>
       </c>
-      <c r="AE134">
+      <c r="AE134" s="1">
         <v>1.1499999761581421</v>
       </c>
-      <c r="AF134">
+      <c r="AF134" s="1">
         <v>0.62999999523162842</v>
       </c>
-      <c r="AG134">
+      <c r="AG134" s="1">
         <v>3.6500000953674316</v>
       </c>
-      <c r="AH134">
+      <c r="AH134" s="1">
         <v>1.0199999809265137</v>
       </c>
     </row>
@@ -14307,16 +14341,16 @@
       <c r="AB135">
         <v>1</v>
       </c>
-      <c r="AC135">
+      <c r="AC135" s="1">
         <v>2.0199999809265137</v>
       </c>
-      <c r="AE135">
+      <c r="AE135" s="1">
         <v>0.27000001072883606</v>
       </c>
-      <c r="AF135">
+      <c r="AF135" s="1">
         <v>1.2400000095367432</v>
       </c>
-      <c r="AH135">
+      <c r="AH135" s="1">
         <v>0.75</v>
       </c>
     </row>
@@ -14405,22 +14439,22 @@
       <c r="AB136">
         <v>2</v>
       </c>
-      <c r="AC136">
+      <c r="AC136" s="1">
         <v>1.7599999904632568</v>
       </c>
-      <c r="AD136">
+      <c r="AD136" s="1">
         <v>3.0499999523162842</v>
       </c>
-      <c r="AE136">
+      <c r="AE136" s="1">
         <v>1.5399999618530273</v>
       </c>
-      <c r="AF136">
+      <c r="AF136" s="1">
         <v>2.119999885559082</v>
       </c>
-      <c r="AG136">
+      <c r="AG136" s="1">
         <v>1.3899999856948853</v>
       </c>
-      <c r="AH136">
+      <c r="AH136" s="1">
         <v>0.86000001430511475</v>
       </c>
     </row>
@@ -14509,22 +14543,22 @@
       <c r="AB137">
         <v>1</v>
       </c>
-      <c r="AC137">
+      <c r="AC137" s="1">
         <v>2.5899999141693115</v>
       </c>
-      <c r="AD137">
+      <c r="AD137" s="1">
         <v>2.619999885559082</v>
       </c>
-      <c r="AE137">
+      <c r="AE137" s="1">
         <v>0.25</v>
       </c>
-      <c r="AF137">
+      <c r="AF137" s="1">
         <v>1.4600000381469727</v>
       </c>
-      <c r="AG137">
+      <c r="AG137" s="1">
         <v>0.9100000262260437</v>
       </c>
-      <c r="AH137">
+      <c r="AH137" s="1">
         <v>0.77999997138977051</v>
       </c>
     </row>
@@ -14613,22 +14647,22 @@
       <c r="AB138">
         <v>2</v>
       </c>
-      <c r="AC138">
+      <c r="AC138" s="1">
         <v>2.059999942779541</v>
       </c>
-      <c r="AD138">
+      <c r="AD138" s="1">
         <v>2.4500000476837158</v>
       </c>
-      <c r="AE138">
+      <c r="AE138" s="1">
         <v>1.75</v>
       </c>
-      <c r="AF138">
+      <c r="AF138" s="1">
         <v>1.059999942779541</v>
       </c>
-      <c r="AG138">
+      <c r="AG138" s="1">
         <v>1.0499999523162842</v>
       </c>
-      <c r="AH138">
+      <c r="AH138" s="1">
         <v>0.81999999284744263</v>
       </c>
     </row>
@@ -14717,22 +14751,22 @@
       <c r="AB139">
         <v>1</v>
       </c>
-      <c r="AC139">
+      <c r="AC139" s="1">
         <v>2.619999885559082</v>
       </c>
-      <c r="AD139">
+      <c r="AD139" s="1">
         <v>2.1400001049041748</v>
       </c>
-      <c r="AE139">
+      <c r="AE139" s="1">
         <v>0.18000000715255737</v>
       </c>
-      <c r="AF139">
+      <c r="AF139" s="1">
         <v>1.0199999809265137</v>
       </c>
-      <c r="AG139">
+      <c r="AG139" s="1">
         <v>1.0800000429153442</v>
       </c>
-      <c r="AH139">
+      <c r="AH139" s="1">
         <v>0.52999997138977051</v>
       </c>
     </row>
@@ -14821,22 +14855,22 @@
       <c r="AB140">
         <v>2</v>
       </c>
-      <c r="AC140">
+      <c r="AC140" s="1">
         <v>0.2199999988079071</v>
       </c>
-      <c r="AD140">
+      <c r="AD140" s="1">
         <v>0.18999999761581421</v>
       </c>
-      <c r="AE140">
+      <c r="AE140" s="1">
         <v>0.43999999761581421</v>
       </c>
-      <c r="AF140">
+      <c r="AF140" s="1">
         <v>0.81000000238418579</v>
       </c>
-      <c r="AG140">
+      <c r="AG140" s="1">
         <v>0.5899999737739563</v>
       </c>
-      <c r="AH140">
+      <c r="AH140" s="1">
         <v>0.73000001907348633</v>
       </c>
     </row>
@@ -14925,22 +14959,22 @@
       <c r="AB141">
         <v>1</v>
       </c>
-      <c r="AC141">
+      <c r="AC141" s="1">
         <v>0.18999999761581421</v>
       </c>
-      <c r="AD141">
+      <c r="AD141" s="1">
         <v>0.8399999737739563</v>
       </c>
-      <c r="AE141">
+      <c r="AE141" s="1">
         <v>0.33000001311302185</v>
       </c>
-      <c r="AF141">
+      <c r="AF141" s="1">
         <v>0.74000000953674316</v>
       </c>
-      <c r="AG141">
+      <c r="AG141" s="1">
         <v>1.1699999570846558</v>
       </c>
-      <c r="AH141">
+      <c r="AH141" s="1">
         <v>1.1499999761581421</v>
       </c>
     </row>
@@ -15029,22 +15063,22 @@
       <c r="AB142">
         <v>2</v>
       </c>
-      <c r="AC142">
+      <c r="AC142" s="1">
         <v>0.40999999642372131</v>
       </c>
-      <c r="AD142">
+      <c r="AD142" s="1">
         <v>1.7000000476837158</v>
       </c>
-      <c r="AE142">
+      <c r="AE142" s="1">
         <v>1.7599999904632568</v>
       </c>
-      <c r="AF142">
+      <c r="AF142" s="1">
         <v>1.2100000381469727</v>
       </c>
-      <c r="AG142">
+      <c r="AG142" s="1">
         <v>1.9299999475479126</v>
       </c>
-      <c r="AH142">
+      <c r="AH142" s="1">
         <v>0.87999999523162842</v>
       </c>
     </row>
@@ -15133,22 +15167,22 @@
       <c r="AB143">
         <v>1</v>
       </c>
-      <c r="AC143">
+      <c r="AC143" s="1">
         <v>1.1499999761581421</v>
       </c>
-      <c r="AD143">
+      <c r="AD143" s="1">
         <v>0.98000001907348633</v>
       </c>
-      <c r="AE143">
+      <c r="AE143" s="1">
         <v>0.38999998569488525</v>
       </c>
-      <c r="AF143">
+      <c r="AF143" s="1">
         <v>0.93000000715255737</v>
       </c>
-      <c r="AG143">
+      <c r="AG143" s="1">
         <v>0.9100000262260437</v>
       </c>
-      <c r="AH143">
+      <c r="AH143" s="1">
         <v>0.72000002861022949</v>
       </c>
     </row>
@@ -15237,22 +15271,22 @@
       <c r="AB144">
         <v>2</v>
       </c>
-      <c r="AC144">
+      <c r="AC144" s="1">
         <v>1.9800000190734863</v>
       </c>
-      <c r="AD144">
+      <c r="AD144" s="1">
         <v>0.2199999988079071</v>
       </c>
-      <c r="AE144">
+      <c r="AE144" s="1">
         <v>0.93999999761581421</v>
       </c>
-      <c r="AF144">
+      <c r="AF144" s="1">
         <v>1.2799999713897705</v>
       </c>
-      <c r="AG144">
+      <c r="AG144" s="1">
         <v>0.77999997138977051</v>
       </c>
-      <c r="AH144">
+      <c r="AH144" s="1">
         <v>0.87999999523162842</v>
       </c>
     </row>
@@ -15341,16 +15375,16 @@
       <c r="AB145">
         <v>1</v>
       </c>
-      <c r="AC145">
+      <c r="AC145" s="1">
         <v>1.4700000286102295</v>
       </c>
-      <c r="AD145">
+      <c r="AD145" s="1">
         <v>1.1399999856948853</v>
       </c>
-      <c r="AF145">
+      <c r="AF145" s="1">
         <v>1.2100000381469727</v>
       </c>
-      <c r="AG145">
+      <c r="AG145" s="1">
         <v>1.1699999570846558</v>
       </c>
     </row>
@@ -15439,22 +15473,22 @@
       <c r="AB146">
         <v>2</v>
       </c>
-      <c r="AC146">
+      <c r="AC146" s="1">
         <v>1.5800000429153442</v>
       </c>
-      <c r="AD146">
+      <c r="AD146" s="1">
         <v>2.8599998950958252</v>
       </c>
-      <c r="AE146">
+      <c r="AE146" s="1">
         <v>0.37999999523162842</v>
       </c>
-      <c r="AF146">
+      <c r="AF146" s="1">
         <v>1.3200000524520874</v>
       </c>
-      <c r="AG146">
+      <c r="AG146" s="1">
         <v>1.6799999475479126</v>
       </c>
-      <c r="AH146">
+      <c r="AH146" s="1">
         <v>0.88999998569488525</v>
       </c>
     </row>
@@ -15543,22 +15577,22 @@
       <c r="AB147">
         <v>1</v>
       </c>
-      <c r="AC147">
+      <c r="AC147" s="1">
         <v>0.44999998807907104</v>
       </c>
-      <c r="AD147">
+      <c r="AD147" s="1">
         <v>0.51999998092651367</v>
       </c>
-      <c r="AE147">
+      <c r="AE147" s="1">
         <v>0.20000000298023224</v>
       </c>
-      <c r="AF147">
+      <c r="AF147" s="1">
         <v>0.63999998569488525</v>
       </c>
-      <c r="AG147">
+      <c r="AG147" s="1">
         <v>0.79000002145767212</v>
       </c>
-      <c r="AH147">
+      <c r="AH147" s="1">
         <v>0.55000001192092896</v>
       </c>
     </row>
@@ -15647,22 +15681,22 @@
       <c r="AB148">
         <v>2</v>
       </c>
-      <c r="AC148">
+      <c r="AC148" s="1">
         <v>1.5099999904632568</v>
       </c>
-      <c r="AD148">
+      <c r="AD148" s="1">
         <v>2.0099999904632568</v>
       </c>
-      <c r="AE148">
+      <c r="AE148" s="1">
         <v>0.51999998092651367</v>
       </c>
-      <c r="AF148">
+      <c r="AF148" s="1">
         <v>1.2599999904632568</v>
       </c>
-      <c r="AG148">
+      <c r="AG148" s="1">
         <v>0.87999999523162842</v>
       </c>
-      <c r="AH148">
+      <c r="AH148" s="1">
         <v>1.1299999952316284</v>
       </c>
     </row>
@@ -15751,22 +15785,22 @@
       <c r="AB149">
         <v>1</v>
       </c>
-      <c r="AC149">
+      <c r="AC149" s="1">
         <v>0.28999999165534973</v>
       </c>
-      <c r="AD149">
+      <c r="AD149" s="1">
         <v>0.34000000357627869</v>
       </c>
-      <c r="AE149">
+      <c r="AE149" s="1">
         <v>0.23999999463558197</v>
       </c>
-      <c r="AF149">
+      <c r="AF149" s="1">
         <v>0.63999998569488525</v>
       </c>
-      <c r="AG149">
+      <c r="AG149" s="1">
         <v>0.85000002384185791</v>
       </c>
-      <c r="AH149">
+      <c r="AH149" s="1">
         <v>0.5899999737739563</v>
       </c>
     </row>
@@ -15855,16 +15889,16 @@
       <c r="AB150">
         <v>2</v>
       </c>
-      <c r="AC150">
+      <c r="AC150" s="1">
         <v>0.2199999988079071</v>
       </c>
-      <c r="AE150">
+      <c r="AE150" s="1">
         <v>0.89999997615814209</v>
       </c>
-      <c r="AF150">
+      <c r="AF150" s="1">
         <v>0.9100000262260437</v>
       </c>
-      <c r="AH150">
+      <c r="AH150" s="1">
         <v>1.1599999666213989</v>
       </c>
     </row>
@@ -15953,22 +15987,22 @@
       <c r="AB151">
         <v>1</v>
       </c>
-      <c r="AC151">
+      <c r="AC151" s="1">
         <v>0.43000000715255737</v>
       </c>
-      <c r="AD151">
+      <c r="AD151" s="1">
         <v>0.40999999642372131</v>
       </c>
-      <c r="AE151">
+      <c r="AE151" s="1">
         <v>0.2199999988079071</v>
       </c>
-      <c r="AF151">
+      <c r="AF151" s="1">
         <v>0.77999997138977051</v>
       </c>
-      <c r="AG151">
+      <c r="AG151" s="1">
         <v>0.82999998331069946</v>
       </c>
-      <c r="AH151">
+      <c r="AH151" s="1">
         <v>0.57999998331069946</v>
       </c>
     </row>
@@ -16057,22 +16091,22 @@
       <c r="AB152">
         <v>2</v>
       </c>
-      <c r="AC152">
+      <c r="AC152" s="1">
         <v>0.36000001430511475</v>
       </c>
-      <c r="AD152">
+      <c r="AD152" s="1">
         <v>0.5899999737739563</v>
       </c>
-      <c r="AE152">
+      <c r="AE152" s="1">
         <v>0.37999999523162842</v>
       </c>
-      <c r="AF152">
+      <c r="AF152" s="1">
         <v>1.0399999618530273</v>
       </c>
-      <c r="AG152">
+      <c r="AG152" s="1">
         <v>0.68999999761581421</v>
       </c>
-      <c r="AH152">
+      <c r="AH152" s="1">
         <v>0.79000002145767212</v>
       </c>
     </row>
@@ -16161,16 +16195,16 @@
       <c r="AB153">
         <v>1</v>
       </c>
-      <c r="AC153">
+      <c r="AC153" s="1">
         <v>1.1799999475479126</v>
       </c>
-      <c r="AD153">
+      <c r="AD153" s="1">
         <v>1.5399999618530273</v>
       </c>
-      <c r="AF153">
+      <c r="AF153" s="1">
         <v>1.3999999761581421</v>
       </c>
-      <c r="AG153">
+      <c r="AG153" s="1">
         <v>1.2599999904632568</v>
       </c>
     </row>
@@ -16259,22 +16293,22 @@
       <c r="AB154">
         <v>2</v>
       </c>
-      <c r="AC154">
+      <c r="AC154" s="1">
         <v>0.86000001430511475</v>
       </c>
-      <c r="AD154">
+      <c r="AD154" s="1">
         <v>0.20999999344348907</v>
       </c>
-      <c r="AE154">
+      <c r="AE154" s="1">
         <v>0.62000000476837158</v>
       </c>
-      <c r="AF154">
+      <c r="AF154" s="1">
         <v>1.2699999809265137</v>
       </c>
-      <c r="AG154">
+      <c r="AG154" s="1">
         <v>0.63999998569488525</v>
       </c>
-      <c r="AH154">
+      <c r="AH154" s="1">
         <v>0.95999997854232788</v>
       </c>
     </row>
@@ -16363,22 +16397,22 @@
       <c r="AB155">
         <v>1</v>
       </c>
-      <c r="AC155">
+      <c r="AC155" s="1">
         <v>1.3400000333786011</v>
       </c>
-      <c r="AD155">
+      <c r="AD155" s="1">
         <v>2.1700000762939453</v>
       </c>
-      <c r="AE155">
+      <c r="AE155" s="1">
         <v>1.1799999475479126</v>
       </c>
-      <c r="AF155">
+      <c r="AF155" s="1">
         <v>0.81999999284744263</v>
       </c>
-      <c r="AG155">
+      <c r="AG155" s="1">
         <v>1.3500000238418579</v>
       </c>
-      <c r="AH155">
+      <c r="AH155" s="1">
         <v>0.50999999046325684</v>
       </c>
     </row>
@@ -16467,22 +16501,22 @@
       <c r="AB156">
         <v>2</v>
       </c>
-      <c r="AC156">
+      <c r="AC156" s="1">
         <v>1.2899999618530273</v>
       </c>
-      <c r="AD156">
+      <c r="AD156" s="1">
         <v>0.55000001192092896</v>
       </c>
-      <c r="AE156">
+      <c r="AE156" s="1">
         <v>0.81999999284744263</v>
       </c>
-      <c r="AF156">
+      <c r="AF156" s="1">
         <v>2.2400000095367432</v>
       </c>
-      <c r="AG156">
+      <c r="AG156" s="1">
         <v>0.8399999737739563</v>
       </c>
-      <c r="AH156">
+      <c r="AH156" s="1">
         <v>0.87999999523162842</v>
       </c>
     </row>
@@ -16571,22 +16605,22 @@
       <c r="AB157">
         <v>1</v>
       </c>
-      <c r="AC157">
+      <c r="AC157" s="1">
         <v>1.75</v>
       </c>
-      <c r="AD157">
+      <c r="AD157" s="1">
         <v>1.6599999666213989</v>
       </c>
-      <c r="AE157">
+      <c r="AE157" s="1">
         <v>0.40999999642372131</v>
       </c>
-      <c r="AF157">
+      <c r="AF157" s="1">
         <v>1.1499999761581421</v>
       </c>
-      <c r="AG157">
+      <c r="AG157" s="1">
         <v>1.1100000143051147</v>
       </c>
-      <c r="AH157">
+      <c r="AH157" s="1">
         <v>0.79000002145767212</v>
       </c>
     </row>
@@ -16675,22 +16709,22 @@
       <c r="AB158">
         <v>2</v>
       </c>
-      <c r="AC158">
+      <c r="AC158" s="1">
         <v>0.47999998927116394</v>
       </c>
-      <c r="AD158">
+      <c r="AD158" s="1">
         <v>2.2899999618530273</v>
       </c>
-      <c r="AE158">
+      <c r="AE158" s="1">
         <v>1.1599999666213989</v>
       </c>
-      <c r="AF158">
+      <c r="AF158" s="1">
         <v>1.1299999952316284</v>
       </c>
-      <c r="AG158">
+      <c r="AG158" s="1">
         <v>1.7599999904632568</v>
       </c>
-      <c r="AH158">
+      <c r="AH158" s="1">
         <v>1.190000057220459</v>
       </c>
     </row>
@@ -16865,22 +16899,22 @@
       <c r="AB160">
         <v>2</v>
       </c>
-      <c r="AC160">
+      <c r="AC160" s="1">
         <v>3.2799999713897705</v>
       </c>
-      <c r="AD160">
+      <c r="AD160" s="1">
         <v>0.94999998807907104</v>
       </c>
-      <c r="AE160">
+      <c r="AE160" s="1">
         <v>0.40999999642372131</v>
       </c>
-      <c r="AF160">
+      <c r="AF160" s="1">
         <v>1.5700000524520874</v>
       </c>
-      <c r="AG160">
+      <c r="AG160" s="1">
         <v>1.6000000238418579</v>
       </c>
-      <c r="AH160">
+      <c r="AH160" s="1">
         <v>0.87000000476837158</v>
       </c>
     </row>
@@ -49704,7 +49738,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62958CC0-5403-4412-9F7C-A43A58ADDD35}">
   <dimension ref="A1:AH161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection sqref="A1:AH161"/>
     </sheetView>
   </sheetViews>
@@ -66573,17 +66607,17 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4CE8736-71CD-443B-A535-A7744CB96E37}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="ce182090-6989-4ee1-a763-8685359d9a12"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="23934a0c-d8ba-4782-9c92-a3b70815aabd"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="23934a0c-d8ba-4782-9c92-a3b70815aabd"/>
-    <ds:schemaRef ds:uri="ce182090-6989-4ee1-a763-8685359d9a12"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
edit - updated script according to the introduction (in the first part of the script) of the column about the first/second decision and relative confidence
</commit_message>
<xml_diff>
--- a/analyses/pilotData_all.xlsx
+++ b/analyses/pilotData_all.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20393"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MMemeo\OneDrive - Fondazione Istituto Italiano Tecnologia\Documents\GitHub\joint-motor-decision\analyses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="8_{DDF43D61-AFCC-4082-8C81-786064A4A95A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{0ECF3D4A-0F7C-415D-88F8-A8CA1D5DB54B}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="8_{DDF43D61-AFCC-4082-8C81-786064A4A95A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{6CA20E88-14ED-4D0A-B0E1-6E67192E1222}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13860" windowHeight="9330" xr2:uid="{A80D8D59-C096-4587-A6C8-4C0B6ECCC775}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13860" windowHeight="9330" activeTab="1" xr2:uid="{A80D8D59-C096-4587-A6C8-4C0B6ECCC775}"/>
   </bookViews>
   <sheets>
     <sheet name="P100" sheetId="1" r:id="rId1"/>
@@ -49,42 +49,6 @@
   </si>
   <si>
     <t>targetLoc</t>
-  </si>
-  <si>
-    <t>A1_decision</t>
-  </si>
-  <si>
-    <t>A1_acc</t>
-  </si>
-  <si>
-    <t>A1_rt</t>
-  </si>
-  <si>
-    <t>A1_mt</t>
-  </si>
-  <si>
-    <t>A1_conf</t>
-  </si>
-  <si>
-    <t>A1_confRT</t>
-  </si>
-  <si>
-    <t>A2_decision</t>
-  </si>
-  <si>
-    <t>A2_acc</t>
-  </si>
-  <si>
-    <t>A2_rt</t>
-  </si>
-  <si>
-    <t>A2_mt</t>
-  </si>
-  <si>
-    <t>A2_conf</t>
-  </si>
-  <si>
-    <t>A2_confRT</t>
   </si>
   <si>
     <t>Coll_decision</t>
@@ -130,6 +94,42 @@
   </si>
   <si>
     <t>mt_finalColl</t>
+  </si>
+  <si>
+    <t>A1_decision</t>
+  </si>
+  <si>
+    <t>A1_acc</t>
+  </si>
+  <si>
+    <t>A1_rt</t>
+  </si>
+  <si>
+    <t>A1_mt</t>
+  </si>
+  <si>
+    <t>A1_conf</t>
+  </si>
+  <si>
+    <t>A1_confRT</t>
+  </si>
+  <si>
+    <t>A2_decision</t>
+  </si>
+  <si>
+    <t>A2_acc</t>
+  </si>
+  <si>
+    <t>A2_rt</t>
+  </si>
+  <si>
+    <t>A2_mt</t>
+  </si>
+  <si>
+    <t>A2_conf</t>
+  </si>
+  <si>
+    <t>A2_confRT</t>
   </si>
 </sst>
 </file>
@@ -484,8 +484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D8BE86-51E1-4E35-A1FE-0679F1EDE2B0}">
   <dimension ref="A1:AH160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AH4" sqref="AH4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,85 +547,85 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>31</v>
+      </c>
+      <c r="R1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S1" t="s">
+        <v>33</v>
+      </c>
+      <c r="T1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="U1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="V1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="W1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="X1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="Y1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Z1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="AA1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="AB1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="W1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
@@ -16927,8 +16927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C94246B-2BAA-4FD1-82A3-919EB16CB05F}">
   <dimension ref="A1:AH160"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16989,85 +16989,85 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>31</v>
+      </c>
+      <c r="R1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S1" t="s">
+        <v>33</v>
+      </c>
+      <c r="T1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="U1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="V1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="W1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="X1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="Y1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Z1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="AA1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="AB1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="W1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
@@ -33400,7 +33400,7 @@
   <dimension ref="A1:AH161"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:AH161"/>
+      <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33428,85 +33428,85 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>31</v>
+      </c>
+      <c r="R1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S1" t="s">
+        <v>33</v>
+      </c>
+      <c r="T1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="U1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="V1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="W1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="X1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="Y1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Z1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="AA1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="AB1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="AC1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="AD1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="AE1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="AF1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="AG1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="AH1" t="s">
         <v>21</v>
-      </c>
-      <c r="W1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
@@ -49738,8 +49738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62958CC0-5403-4412-9F7C-A43A58ADDD35}">
   <dimension ref="A1:AH161"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection sqref="A1:AH161"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49767,85 +49767,85 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>31</v>
+      </c>
+      <c r="R1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S1" t="s">
+        <v>33</v>
+      </c>
+      <c r="T1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="U1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="V1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="W1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="X1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="Y1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Z1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="AA1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="AB1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="W1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
@@ -66607,16 +66607,16 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4CE8736-71CD-443B-A535-A7744CB96E37}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="23934a0c-d8ba-4782-9c92-a3b70815aabd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="ce182090-6989-4ee1-a763-8685359d9a12"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="23934a0c-d8ba-4782-9c92-a3b70815aabd"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>

</xml_diff>